<commit_message>
Paper's figures generating files
</commit_message>
<xml_diff>
--- a/results/Paper/table_4.xlsx
+++ b/results/Paper/table_4.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9766F1EC-F06E-4666-84B1-65ACBEF9FCA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2BB2A3-D236-4A0B-8B5D-6BDB4FA48B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LTMLE" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="0" r:id="rId6"/>
+    <pivotCache cacheId="1" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -765,7 +765,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -790,19 +790,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="2"/>
     </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -2252,7 +2251,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable29" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable29" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
   <location ref="N4:O47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
@@ -7378,8 +7377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView zoomScale="115" workbookViewId="0">
-      <selection activeCell="L2" sqref="L2"/>
+    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
+      <selection activeCell="Q22" sqref="Q22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7630,7 +7629,7 @@
       <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5" s="16">
+      <c r="O5">
         <v>0.38408227893435404</v>
       </c>
     </row>
@@ -7682,7 +7681,7 @@
       <c r="N6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O6" s="16">
+      <c r="O6">
         <v>0.48164705582437051</v>
       </c>
     </row>
@@ -7734,7 +7733,7 @@
       <c r="N7" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O7" s="16">
+      <c r="O7">
         <v>0.51160443995962901</v>
       </c>
     </row>
@@ -7786,7 +7785,7 @@
       <c r="N8" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8">
         <v>0.451689671689112</v>
       </c>
     </row>
@@ -7838,7 +7837,7 @@
       <c r="N9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9">
         <v>0.28651750204433751</v>
       </c>
     </row>
@@ -7890,7 +7889,7 @@
       <c r="N10" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10">
         <v>0.28655959425226002</v>
       </c>
     </row>
@@ -7942,7 +7941,7 @@
       <c r="N11" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11">
         <v>0.28647540983641501</v>
       </c>
     </row>
@@ -7994,7 +7993,7 @@
       <c r="N12" s="9" t="s">
         <v>43</v>
       </c>
-      <c r="O12" s="16">
+      <c r="O12">
         <v>0.37191644982658001</v>
       </c>
     </row>
@@ -8046,7 +8045,7 @@
       <c r="N13" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O13" s="16">
+      <c r="O13">
         <v>0.59614733495410555</v>
       </c>
     </row>
@@ -8098,7 +8097,7 @@
       <c r="N14" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14">
         <v>0.61925795053003196</v>
       </c>
     </row>
@@ -8150,7 +8149,7 @@
       <c r="N15" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15">
         <v>0.57303671937817902</v>
       </c>
     </row>
@@ -8202,7 +8201,7 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16">
         <v>0.1476855646990545</v>
       </c>
     </row>
@@ -8254,7 +8253,7 @@
       <c r="N17" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O17" s="16">
+      <c r="O17">
         <v>0.1321499013812</v>
       </c>
     </row>
@@ -8306,7 +8305,7 @@
       <c r="N18" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O18" s="16">
+      <c r="O18">
         <v>0.163221228016909</v>
       </c>
     </row>
@@ -8358,7 +8357,7 @@
       <c r="N19" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="O19" s="16">
+      <c r="O19">
         <v>0.46311959728281249</v>
       </c>
     </row>
@@ -8410,7 +8409,7 @@
       <c r="N20" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20">
         <v>0.69002365571811208</v>
       </c>
     </row>
@@ -8462,7 +8461,7 @@
       <c r="N21" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21">
         <v>0.66896551724132902</v>
       </c>
     </row>
@@ -8514,7 +8513,7 @@
       <c r="N22" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22">
         <v>0.71108179419489503</v>
       </c>
     </row>
@@ -8566,7 +8565,7 @@
       <c r="N23" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O23" s="16">
+      <c r="O23">
         <v>0.23621553884751301</v>
       </c>
     </row>
@@ -8618,7 +8617,7 @@
       <c r="N24" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O24" s="16">
+      <c r="O24">
         <v>0.21491228070193999</v>
       </c>
     </row>
@@ -8670,7 +8669,7 @@
       <c r="N25" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O25" s="16">
+      <c r="O25">
         <v>0.257518796993086</v>
       </c>
     </row>
@@ -8722,7 +8721,7 @@
       <c r="N26" s="9" t="s">
         <v>44</v>
       </c>
-      <c r="O26" s="16">
+      <c r="O26">
         <v>0.37006554197770503</v>
       </c>
     </row>
@@ -8774,7 +8773,7 @@
       <c r="N27" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O27" s="16">
+      <c r="O27">
         <v>0.51531660251544653</v>
       </c>
     </row>
@@ -8826,7 +8825,7 @@
       <c r="N28" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O28" s="16">
+      <c r="O28">
         <v>0.54324644544899903</v>
       </c>
     </row>
@@ -8878,7 +8877,7 @@
       <c r="N29" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O29" s="16">
+      <c r="O29">
         <v>0.48738675958189398</v>
       </c>
     </row>
@@ -8930,7 +8929,7 @@
       <c r="N30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O30" s="16">
+      <c r="O30">
         <v>0.22481448143996349</v>
       </c>
     </row>
@@ -8982,7 +8981,7 @@
       <c r="N31" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O31" s="16">
+      <c r="O31">
         <v>0.215393452039258</v>
       </c>
     </row>
@@ -9034,7 +9033,7 @@
       <c r="N32" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O32" s="16">
+      <c r="O32">
         <v>0.23423551084066899</v>
       </c>
     </row>
@@ -9086,7 +9085,7 @@
       <c r="N33" s="9" t="s">
         <v>25</v>
       </c>
-      <c r="O33" s="16">
+      <c r="O33">
         <v>0.3935388940891873</v>
       </c>
     </row>
@@ -9138,7 +9137,7 @@
       <c r="N34" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O34" s="16">
+      <c r="O34">
         <v>0.49365482001656452</v>
       </c>
     </row>
@@ -9190,7 +9189,7 @@
       <c r="N35" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O35" s="16">
+      <c r="O35">
         <v>0.52089407191416504</v>
       </c>
     </row>
@@ -9242,7 +9241,7 @@
       <c r="N36" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O36" s="16">
+      <c r="O36">
         <v>0.46641556811896401</v>
       </c>
     </row>
@@ -9294,7 +9293,7 @@
       <c r="N37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O37" s="16">
+      <c r="O37">
         <v>0.29342296816181002</v>
       </c>
     </row>
@@ -9346,7 +9345,7 @@
       <c r="N38" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O38" s="16">
+      <c r="O38">
         <v>0.29179566563500697</v>
       </c>
     </row>
@@ -9398,7 +9397,7 @@
       <c r="N39" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O39" s="16">
+      <c r="O39">
         <v>0.295050270688613</v>
       </c>
     </row>
@@ -9450,7 +9449,7 @@
       <c r="N40" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="O40" s="16">
+      <c r="O40">
         <v>0.35730962902056324</v>
       </c>
     </row>
@@ -9502,7 +9501,7 @@
       <c r="N41" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O41" s="16">
+      <c r="O41">
         <v>0.59359143492087996</v>
       </c>
     </row>
@@ -9554,7 +9553,7 @@
       <c r="N42" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O42" s="16">
+      <c r="O42">
         <v>0.61425959780623896</v>
       </c>
     </row>
@@ -9606,7 +9605,7 @@
       <c r="N43" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O43" s="16">
+      <c r="O43">
         <v>0.57292327203552096</v>
       </c>
     </row>
@@ -9658,7 +9657,7 @@
       <c r="N44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O44" s="16">
+      <c r="O44">
         <v>0.12102782312024651</v>
       </c>
     </row>
@@ -9710,7 +9709,7 @@
       <c r="N45" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="O45" s="16">
+      <c r="O45">
         <v>0.106077348512377</v>
       </c>
     </row>
@@ -9762,7 +9761,7 @@
       <c r="N46" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="O46" s="16">
+      <c r="O46">
         <v>0.13597829772811601</v>
       </c>
     </row>
@@ -9814,7 +9813,7 @@
       <c r="N47" s="9" t="s">
         <v>47</v>
       </c>
-      <c r="O47" s="16">
+      <c r="O47">
         <v>0.390005398521867</v>
       </c>
     </row>
@@ -13219,18 +13218,18 @@
   <sheetData>
     <row r="3" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="13" t="s">
+      <c r="D3" s="14"/>
+      <c r="E3" s="14"/>
+      <c r="F3" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="13"/>
+      <c r="G3" s="15"/>
+      <c r="H3" s="15"/>
+      <c r="I3" s="15"/>
+      <c r="J3" s="15"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -13269,10 +13268,10 @@
     </row>
     <row r="5" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="14" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -13301,8 +13300,8 @@
     </row>
     <row r="6" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="13"/>
-      <c r="D6" s="15"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="13"/>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
@@ -13329,8 +13328,8 @@
     </row>
     <row r="7" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="C7" s="13"/>
-      <c r="D7" s="14" t="s">
+      <c r="C7" s="15"/>
+      <c r="D7" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -13359,8 +13358,8 @@
     </row>
     <row r="8" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="C8" s="13"/>
-      <c r="D8" s="15"/>
+      <c r="C8" s="15"/>
+      <c r="D8" s="13"/>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
@@ -13387,10 +13386,10 @@
     </row>
     <row r="9" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="14" t="s">
+      <c r="D9" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -13419,8 +13418,8 @@
     </row>
     <row r="10" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="C10" s="13"/>
-      <c r="D10" s="15"/>
+      <c r="C10" s="15"/>
+      <c r="D10" s="13"/>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
@@ -13447,8 +13446,8 @@
     </row>
     <row r="11" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="C11" s="13"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="15"/>
+      <c r="D11" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -13477,8 +13476,8 @@
     </row>
     <row r="12" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="15"/>
+      <c r="C12" s="15"/>
+      <c r="D12" s="13"/>
       <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
@@ -13505,10 +13504,10 @@
     </row>
     <row r="13" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="14" t="s">
+      <c r="D13" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -13537,8 +13536,8 @@
     </row>
     <row r="14" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="15"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="13"/>
       <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
@@ -13565,8 +13564,8 @@
     </row>
     <row r="15" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="13"/>
-      <c r="D15" s="14" t="s">
+      <c r="C15" s="15"/>
+      <c r="D15" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -13595,8 +13594,8 @@
     </row>
     <row r="16" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="15"/>
+      <c r="C16" s="15"/>
+      <c r="D16" s="13"/>
       <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
@@ -13623,10 +13622,10 @@
     </row>
     <row r="17" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="14" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -13655,8 +13654,8 @@
     </row>
     <row r="18" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="13"/>
-      <c r="D18" s="15"/>
+      <c r="C18" s="15"/>
+      <c r="D18" s="13"/>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
@@ -13683,8 +13682,8 @@
     </row>
     <row r="19" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="15"/>
+      <c r="D19" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -13713,8 +13712,8 @@
     </row>
     <row r="20" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="15"/>
+      <c r="C20" s="15"/>
+      <c r="D20" s="13"/>
       <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
@@ -13741,10 +13740,10 @@
     </row>
     <row r="21" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-      <c r="C21" s="13" t="s">
+      <c r="C21" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="14" t="s">
+      <c r="D21" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -13773,8 +13772,8 @@
     </row>
     <row r="22" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-      <c r="C22" s="13"/>
-      <c r="D22" s="15"/>
+      <c r="C22" s="15"/>
+      <c r="D22" s="13"/>
       <c r="E22" s="4" t="s">
         <v>11</v>
       </c>
@@ -13801,8 +13800,8 @@
     </row>
     <row r="23" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="C23" s="13"/>
-      <c r="D23" s="14" t="s">
+      <c r="C23" s="15"/>
+      <c r="D23" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -13831,8 +13830,8 @@
     </row>
     <row r="24" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="C24" s="13"/>
-      <c r="D24" s="15"/>
+      <c r="C24" s="15"/>
+      <c r="D24" s="13"/>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
@@ -13859,10 +13858,10 @@
     </row>
     <row r="25" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="14" t="s">
+      <c r="D25" s="12" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -13891,8 +13890,8 @@
     </row>
     <row r="26" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
-      <c r="C26" s="13"/>
-      <c r="D26" s="15"/>
+      <c r="C26" s="15"/>
+      <c r="D26" s="13"/>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
@@ -13919,8 +13918,8 @@
     </row>
     <row r="27" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
-      <c r="C27" s="13"/>
-      <c r="D27" s="14" t="s">
+      <c r="C27" s="15"/>
+      <c r="D27" s="12" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -13949,8 +13948,8 @@
     </row>
     <row r="28" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
-      <c r="C28" s="13"/>
-      <c r="D28" s="15"/>
+      <c r="C28" s="15"/>
+      <c r="D28" s="13"/>
       <c r="E28" s="4" t="s">
         <v>11</v>
       </c>
@@ -14172,11 +14171,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C17:C20"/>
@@ -14192,6 +14186,11 @@
     <mergeCell ref="D19:D20"/>
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="D13:D14"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14202,8 +14201,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{49F68BBC-1C6E-44E2-9561-9966A635774D}">
   <dimension ref="A1:Q121"/>
   <sheetViews>
-    <sheetView topLeftCell="A85" workbookViewId="0">
-      <selection activeCell="I119" sqref="I119"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:J1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14407,23 +14406,23 @@
         <v>0</v>
       </c>
       <c r="L4">
-        <f t="shared" ref="L4:L35" si="0">IFERROR(G4/G5,0)</f>
+        <f t="shared" ref="L4" si="0">IFERROR(G4/G5,0)</f>
         <v>0.98913313936878433</v>
       </c>
       <c r="M4">
-        <f t="shared" ref="M4:M35" si="1">IFERROR(H4/H5, 0)</f>
+        <f t="shared" ref="M4" si="1">IFERROR(H4/H5, 0)</f>
         <v>1.021163568989035</v>
       </c>
       <c r="N4">
-        <f t="shared" ref="N4:N35" si="2">IFERROR(I4/I5, 0)</f>
+        <f t="shared" ref="N4" si="2">IFERROR(I4/I5, 0)</f>
         <v>0.96070695596641598</v>
       </c>
       <c r="O4">
-        <f t="shared" ref="O4:O35" si="3">IFERROR(J4/J5, 0)</f>
+        <f t="shared" ref="O4" si="3">IFERROR(J4/J5, 0)</f>
         <v>0</v>
       </c>
       <c r="Q4" t="str">
-        <f t="shared" ref="Q4:Q35" si="4">_xlfn.CONCAT(ROUND(L4, 2), " (", ROUND(N4,2), " - ", ROUND(M4,2),  ")", IF(AND(O4 &lt;0.05, NOT(ISBLANK(O4))), "*", " ") )</f>
+        <f t="shared" ref="Q4" si="4">_xlfn.CONCAT(ROUND(L4, 2), " (", ROUND(N4,2), " - ", ROUND(M4,2),  ")", IF(AND(O4 &lt;0.05, NOT(ISBLANK(O4))), "*", " ") )</f>
         <v>0.99 (0.96 - 1.02)*</v>
       </c>
     </row>
@@ -14511,23 +14510,23 @@
         <v>1.5247713908139899E-288</v>
       </c>
       <c r="L6">
-        <f t="shared" ref="L6:L37" si="5">IFERROR(G6/G7,0)</f>
+        <f t="shared" ref="L6" si="5">IFERROR(G6/G7,0)</f>
         <v>0.86008736587734891</v>
       </c>
       <c r="M6">
-        <f t="shared" ref="M6:M37" si="6">IFERROR(H6/H7, 0)</f>
+        <f t="shared" ref="M6" si="6">IFERROR(H6/H7, 0)</f>
         <v>0.91201173800737678</v>
       </c>
       <c r="N6">
-        <f t="shared" ref="N6:N37" si="7">IFERROR(I6/I7, 0)</f>
+        <f t="shared" ref="N6" si="7">IFERROR(I6/I7, 0)</f>
         <v>0.81827283178897692</v>
       </c>
       <c r="O6">
-        <f t="shared" ref="O6:O37" si="8">IFERROR(J6/J7, 0)</f>
+        <f t="shared" ref="O6" si="8">IFERROR(J6/J7, 0)</f>
         <v>1.801564479619643E-215</v>
       </c>
       <c r="Q6" t="str">
-        <f t="shared" ref="Q6:Q37" si="9">_xlfn.CONCAT(ROUND(L6, 2), " (", ROUND(N6,2), " - ", ROUND(M6,2),  ")", IF(AND(O6 &lt;0.05, NOT(ISBLANK(O6))), "*", " ") )</f>
+        <f t="shared" ref="Q6" si="9">_xlfn.CONCAT(ROUND(L6, 2), " (", ROUND(N6,2), " - ", ROUND(M6,2),  ")", IF(AND(O6 &lt;0.05, NOT(ISBLANK(O6))), "*", " ") )</f>
         <v>0.86 (0.82 - 0.91)*</v>
       </c>
     </row>
@@ -14615,23 +14614,23 @@
         <v>0</v>
       </c>
       <c r="L8">
-        <f t="shared" ref="L8:L39" si="10">IFERROR(G8/G9,0)</f>
+        <f t="shared" ref="L8" si="10">IFERROR(G8/G9,0)</f>
         <v>1.0451521231965006</v>
       </c>
       <c r="M8">
-        <f t="shared" ref="M8:M39" si="11">IFERROR(H8/H9, 0)</f>
+        <f t="shared" ref="M8" si="11">IFERROR(H8/H9, 0)</f>
         <v>1.1152843831263437</v>
       </c>
       <c r="N8">
-        <f t="shared" ref="N8:N39" si="12">IFERROR(I8/I9, 0)</f>
+        <f t="shared" ref="N8" si="12">IFERROR(I8/I9, 0)</f>
         <v>0.98901130651854641</v>
       </c>
       <c r="O8">
-        <f t="shared" ref="O8:O39" si="13">IFERROR(J8/J9, 0)</f>
+        <f t="shared" ref="O8" si="13">IFERROR(J8/J9, 0)</f>
         <v>0</v>
       </c>
       <c r="Q8" t="str">
-        <f t="shared" ref="Q8:Q39" si="14">_xlfn.CONCAT(ROUND(L8, 2), " (", ROUND(N8,2), " - ", ROUND(M8,2),  ")", IF(AND(O8 &lt;0.05, NOT(ISBLANK(O8))), "*", " ") )</f>
+        <f t="shared" ref="Q8" si="14">_xlfn.CONCAT(ROUND(L8, 2), " (", ROUND(N8,2), " - ", ROUND(M8,2),  ")", IF(AND(O8 &lt;0.05, NOT(ISBLANK(O8))), "*", " ") )</f>
         <v>1.05 (0.99 - 1.12)*</v>
       </c>
     </row>
@@ -14719,23 +14718,23 @@
         <v>0</v>
       </c>
       <c r="L10">
-        <f t="shared" ref="L10:L41" si="15">IFERROR(G10/G11,0)</f>
+        <f t="shared" ref="L10" si="15">IFERROR(G10/G11,0)</f>
         <v>0.88288849042192652</v>
       </c>
       <c r="M10">
-        <f t="shared" ref="M10:M41" si="16">IFERROR(H10/H11, 0)</f>
+        <f t="shared" ref="M10" si="16">IFERROR(H10/H11, 0)</f>
         <v>0.90875953848640567</v>
       </c>
       <c r="N10">
-        <f t="shared" ref="N10:N41" si="17">IFERROR(I10/I11, 0)</f>
+        <f t="shared" ref="N10" si="17">IFERROR(I10/I11, 0)</f>
         <v>0.85998464939472907</v>
       </c>
       <c r="O10">
-        <f t="shared" ref="O10:O41" si="18">IFERROR(J10/J11, 0)</f>
+        <f t="shared" ref="O10" si="18">IFERROR(J10/J11, 0)</f>
         <v>0</v>
       </c>
       <c r="Q10" t="str">
-        <f t="shared" ref="Q10:Q41" si="19">_xlfn.CONCAT(ROUND(L10, 2), " (", ROUND(N10,2), " - ", ROUND(M10,2),  ")", IF(AND(O10 &lt;0.05, NOT(ISBLANK(O10))), "*", " ") )</f>
+        <f t="shared" ref="Q10" si="19">_xlfn.CONCAT(ROUND(L10, 2), " (", ROUND(N10,2), " - ", ROUND(M10,2),  ")", IF(AND(O10 &lt;0.05, NOT(ISBLANK(O10))), "*", " ") )</f>
         <v>0.88 (0.86 - 0.91)*</v>
       </c>
     </row>
@@ -14823,23 +14822,23 @@
         <v>0</v>
       </c>
       <c r="L12">
-        <f t="shared" ref="L12:L43" si="20">IFERROR(G12/G13,0)</f>
+        <f t="shared" ref="L12" si="20">IFERROR(G12/G13,0)</f>
         <v>0.99970622370517837</v>
       </c>
       <c r="M12">
-        <f t="shared" ref="M12:M43" si="21">IFERROR(H12/H13, 0)</f>
+        <f t="shared" ref="M12" si="21">IFERROR(H12/H13, 0)</f>
         <v>1.0498375895785585</v>
       </c>
       <c r="N12">
-        <f t="shared" ref="N12:N43" si="22">IFERROR(I12/I13, 0)</f>
+        <f t="shared" ref="N12" si="22">IFERROR(I12/I13, 0)</f>
         <v>0.95784653781059326</v>
       </c>
       <c r="O12">
-        <f t="shared" ref="O12:O43" si="23">IFERROR(J12/J13, 0)</f>
+        <f t="shared" ref="O12" si="23">IFERROR(J12/J13, 0)</f>
         <v>0</v>
       </c>
       <c r="Q12" t="str">
-        <f t="shared" ref="Q12:Q43" si="24">_xlfn.CONCAT(ROUND(L12, 2), " (", ROUND(N12,2), " - ", ROUND(M12,2),  ")", IF(AND(O12 &lt;0.05, NOT(ISBLANK(O12))), "*", " ") )</f>
+        <f t="shared" ref="Q12" si="24">_xlfn.CONCAT(ROUND(L12, 2), " (", ROUND(N12,2), " - ", ROUND(M12,2),  ")", IF(AND(O12 &lt;0.05, NOT(ISBLANK(O12))), "*", " ") )</f>
         <v>1 (0.96 - 1.05)*</v>
       </c>
     </row>
@@ -14927,23 +14926,23 @@
         <v>0</v>
       </c>
       <c r="L14">
-        <f t="shared" ref="L14:L45" si="25">IFERROR(G14/G15,0)</f>
+        <f t="shared" ref="L14" si="25">IFERROR(G14/G15,0)</f>
         <v>1.0110476578030458</v>
       </c>
       <c r="M14">
-        <f t="shared" ref="M14:M45" si="26">IFERROR(H14/H15, 0)</f>
+        <f t="shared" ref="M14" si="26">IFERROR(H14/H15, 0)</f>
         <v>1.0423693731415129</v>
       </c>
       <c r="N14">
-        <f t="shared" ref="N14:N45" si="27">IFERROR(I14/I15, 0)</f>
+        <f t="shared" ref="N14" si="27">IFERROR(I14/I15, 0)</f>
         <v>0.98341386840112466</v>
       </c>
       <c r="O14">
-        <f t="shared" ref="O14:O45" si="28">IFERROR(J14/J15, 0)</f>
+        <f t="shared" ref="O14" si="28">IFERROR(J14/J15, 0)</f>
         <v>0</v>
       </c>
       <c r="Q14" t="str">
-        <f t="shared" ref="Q14:Q45" si="29">_xlfn.CONCAT(ROUND(L14, 2), " (", ROUND(N14,2), " - ", ROUND(M14,2),  ")", IF(AND(O14 &lt;0.05, NOT(ISBLANK(O14))), "*", " ") )</f>
+        <f t="shared" ref="Q14" si="29">_xlfn.CONCAT(ROUND(L14, 2), " (", ROUND(N14,2), " - ", ROUND(M14,2),  ")", IF(AND(O14 &lt;0.05, NOT(ISBLANK(O14))), "*", " ") )</f>
         <v>1.01 (0.98 - 1.04)*</v>
       </c>
     </row>
@@ -15031,23 +15030,23 @@
         <v>1.0687423870702899E-278</v>
       </c>
       <c r="L16">
-        <f t="shared" ref="L16:L47" si="30">IFERROR(G16/G17,0)</f>
+        <f t="shared" ref="L16" si="30">IFERROR(G16/G17,0)</f>
         <v>0.94680010183053276</v>
       </c>
       <c r="M16">
-        <f t="shared" ref="M16:M47" si="31">IFERROR(H16/H17, 0)</f>
+        <f t="shared" ref="M16" si="31">IFERROR(H16/H17, 0)</f>
         <v>0.99438252639995151</v>
       </c>
       <c r="N16">
-        <f t="shared" ref="N16:N47" si="32">IFERROR(I16/I17, 0)</f>
+        <f t="shared" ref="N16" si="32">IFERROR(I16/I17, 0)</f>
         <v>0.90788207376495345</v>
       </c>
       <c r="O16">
-        <f t="shared" ref="O16:O47" si="33">IFERROR(J16/J17, 0)</f>
+        <f t="shared" ref="O16" si="33">IFERROR(J16/J17, 0)</f>
         <v>3.6282992833310727E-194</v>
       </c>
       <c r="Q16" t="str">
-        <f t="shared" ref="Q16:Q47" si="34">_xlfn.CONCAT(ROUND(L16, 2), " (", ROUND(N16,2), " - ", ROUND(M16,2),  ")", IF(AND(O16 &lt;0.05, NOT(ISBLANK(O16))), "*", " ") )</f>
+        <f t="shared" ref="Q16" si="34">_xlfn.CONCAT(ROUND(L16, 2), " (", ROUND(N16,2), " - ", ROUND(M16,2),  ")", IF(AND(O16 &lt;0.05, NOT(ISBLANK(O16))), "*", " ") )</f>
         <v>0.95 (0.91 - 0.99)*</v>
       </c>
     </row>
@@ -15135,23 +15134,23 @@
         <v>3.17920637696875E-251</v>
       </c>
       <c r="L18">
-        <f t="shared" ref="L18:L49" si="35">IFERROR(G18/G19,0)</f>
+        <f t="shared" ref="L18" si="35">IFERROR(G18/G19,0)</f>
         <v>1.0336696643999663</v>
       </c>
       <c r="M18">
-        <f t="shared" ref="M18:M49" si="36">IFERROR(H18/H19, 0)</f>
+        <f t="shared" ref="M18" si="36">IFERROR(H18/H19, 0)</f>
         <v>1.0898721784694567</v>
       </c>
       <c r="N18">
-        <f t="shared" ref="N18:N49" si="37">IFERROR(I18/I19, 0)</f>
+        <f t="shared" ref="N18" si="37">IFERROR(I18/I19, 0)</f>
         <v>0.9882839807425452</v>
       </c>
       <c r="O18">
-        <f t="shared" ref="O18:O49" si="38">IFERROR(J18/J19, 0)</f>
+        <f t="shared" ref="O18" si="38">IFERROR(J18/J19, 0)</f>
         <v>2.7718956504632462E-176</v>
       </c>
       <c r="Q18" t="str">
-        <f t="shared" ref="Q18:Q49" si="39">_xlfn.CONCAT(ROUND(L18, 2), " (", ROUND(N18,2), " - ", ROUND(M18,2),  ")", IF(AND(O18 &lt;0.05, NOT(ISBLANK(O18))), "*", " ") )</f>
+        <f t="shared" ref="Q18" si="39">_xlfn.CONCAT(ROUND(L18, 2), " (", ROUND(N18,2), " - ", ROUND(M18,2),  ")", IF(AND(O18 &lt;0.05, NOT(ISBLANK(O18))), "*", " ") )</f>
         <v>1.03 (0.99 - 1.09)*</v>
       </c>
     </row>
@@ -15239,23 +15238,23 @@
         <v>8.45164143897459E-74</v>
       </c>
       <c r="L20">
-        <f t="shared" ref="L20:L51" si="40">IFERROR(G20/G21,0)</f>
+        <f t="shared" ref="L20" si="40">IFERROR(G20/G21,0)</f>
         <v>1.1111111111105882</v>
       </c>
       <c r="M20">
-        <f t="shared" ref="M20:M51" si="41">IFERROR(H20/H21, 0)</f>
+        <f t="shared" ref="M20" si="41">IFERROR(H20/H21, 0)</f>
         <v>1.4058798320176662</v>
       </c>
       <c r="N20">
-        <f t="shared" ref="N20:N51" si="42">IFERROR(I20/I21, 0)</f>
+        <f t="shared" ref="N20" si="42">IFERROR(I20/I21, 0)</f>
         <v>0.95060559104225184</v>
       </c>
       <c r="O20">
-        <f t="shared" ref="O20:O51" si="43">IFERROR(J20/J21, 0)</f>
+        <f t="shared" ref="O20" si="43">IFERROR(J20/J21, 0)</f>
         <v>2.8074325514972177E-63</v>
       </c>
       <c r="Q20" t="str">
-        <f t="shared" ref="Q20:Q51" si="44">_xlfn.CONCAT(ROUND(L20, 2), " (", ROUND(N20,2), " - ", ROUND(M20,2),  ")", IF(AND(O20 &lt;0.05, NOT(ISBLANK(O20))), "*", " ") )</f>
+        <f t="shared" ref="Q20" si="44">_xlfn.CONCAT(ROUND(L20, 2), " (", ROUND(N20,2), " - ", ROUND(M20,2),  ")", IF(AND(O20 &lt;0.05, NOT(ISBLANK(O20))), "*", " ") )</f>
         <v>1.11 (0.95 - 1.41)*</v>
       </c>
     </row>
@@ -15343,23 +15342,23 @@
         <v>0</v>
       </c>
       <c r="L22">
-        <f t="shared" ref="L22:L53" si="45">IFERROR(G22/G23,0)</f>
+        <f t="shared" ref="L22" si="45">IFERROR(G22/G23,0)</f>
         <v>0.92878866191831111</v>
       </c>
       <c r="M22">
-        <f t="shared" ref="M22:M53" si="46">IFERROR(H22/H23, 0)</f>
+        <f t="shared" ref="M22" si="46">IFERROR(H22/H23, 0)</f>
         <v>0.9430419631429765</v>
       </c>
       <c r="N22">
-        <f t="shared" ref="N22:N53" si="47">IFERROR(I22/I23, 0)</f>
+        <f t="shared" ref="N22" si="47">IFERROR(I22/I23, 0)</f>
         <v>0.91545906662900145</v>
       </c>
       <c r="O22">
-        <f t="shared" ref="O22:O53" si="48">IFERROR(J22/J23, 0)</f>
+        <f t="shared" ref="O22" si="48">IFERROR(J22/J23, 0)</f>
         <v>0</v>
       </c>
       <c r="Q22" t="str">
-        <f t="shared" ref="Q22:Q53" si="49">_xlfn.CONCAT(ROUND(L22, 2), " (", ROUND(N22,2), " - ", ROUND(M22,2),  ")", IF(AND(O22 &lt;0.05, NOT(ISBLANK(O22))), "*", " ") )</f>
+        <f t="shared" ref="Q22" si="49">_xlfn.CONCAT(ROUND(L22, 2), " (", ROUND(N22,2), " - ", ROUND(M22,2),  ")", IF(AND(O22 &lt;0.05, NOT(ISBLANK(O22))), "*", " ") )</f>
         <v>0.93 (0.92 - 0.94)*</v>
       </c>
     </row>
@@ -15447,23 +15446,23 @@
         <v>0</v>
       </c>
       <c r="L24">
-        <f t="shared" ref="L24:L55" si="50">IFERROR(G24/G25,0)</f>
+        <f t="shared" ref="L24" si="50">IFERROR(G24/G25,0)</f>
         <v>1.1284886860113814</v>
       </c>
       <c r="M24">
-        <f t="shared" ref="M24:M55" si="51">IFERROR(H24/H25, 0)</f>
+        <f t="shared" ref="M24" si="51">IFERROR(H24/H25, 0)</f>
         <v>1.1971347398672327</v>
       </c>
       <c r="N24">
-        <f t="shared" ref="N24:N55" si="52">IFERROR(I24/I25, 0)</f>
+        <f t="shared" ref="N24" si="52">IFERROR(I24/I25, 0)</f>
         <v>1.0723340884236823</v>
       </c>
       <c r="O24">
-        <f t="shared" ref="O24:O55" si="53">IFERROR(J24/J25, 0)</f>
+        <f t="shared" ref="O24" si="53">IFERROR(J24/J25, 0)</f>
         <v>0</v>
       </c>
       <c r="Q24" t="str">
-        <f t="shared" ref="Q24:Q55" si="54">_xlfn.CONCAT(ROUND(L24, 2), " (", ROUND(N24,2), " - ", ROUND(M24,2),  ")", IF(AND(O24 &lt;0.05, NOT(ISBLANK(O24))), "*", " ") )</f>
+        <f t="shared" ref="Q24" si="54">_xlfn.CONCAT(ROUND(L24, 2), " (", ROUND(N24,2), " - ", ROUND(M24,2),  ")", IF(AND(O24 &lt;0.05, NOT(ISBLANK(O24))), "*", " ") )</f>
         <v>1.13 (1.07 - 1.2)*</v>
       </c>
     </row>
@@ -15551,23 +15550,23 @@
         <v>0</v>
       </c>
       <c r="L26">
-        <f t="shared" ref="L26:L57" si="55">IFERROR(G26/G27,0)</f>
+        <f t="shared" ref="L26" si="55">IFERROR(G26/G27,0)</f>
         <v>0.95554700512895863</v>
       </c>
       <c r="M26">
-        <f t="shared" ref="M26:M57" si="56">IFERROR(H26/H27, 0)</f>
+        <f t="shared" ref="M26" si="56">IFERROR(H26/H27, 0)</f>
         <v>0.98015039498809331</v>
       </c>
       <c r="N26">
-        <f t="shared" ref="N26:N57" si="57">IFERROR(I26/I27, 0)</f>
+        <f t="shared" ref="N26" si="57">IFERROR(I26/I27, 0)</f>
         <v>0.93332157263150484</v>
       </c>
       <c r="O26">
-        <f t="shared" ref="O26:O57" si="58">IFERROR(J26/J27, 0)</f>
+        <f t="shared" ref="O26" si="58">IFERROR(J26/J27, 0)</f>
         <v>0</v>
       </c>
       <c r="Q26" t="str">
-        <f t="shared" ref="Q26:Q57" si="59">_xlfn.CONCAT(ROUND(L26, 2), " (", ROUND(N26,2), " - ", ROUND(M26,2),  ")", IF(AND(O26 &lt;0.05, NOT(ISBLANK(O26))), "*", " ") )</f>
+        <f t="shared" ref="Q26" si="59">_xlfn.CONCAT(ROUND(L26, 2), " (", ROUND(N26,2), " - ", ROUND(M26,2),  ")", IF(AND(O26 &lt;0.05, NOT(ISBLANK(O26))), "*", " ") )</f>
         <v>0.96 (0.93 - 0.98)*</v>
       </c>
     </row>
@@ -15655,23 +15654,23 @@
         <v>5.8598858583285003E-252</v>
       </c>
       <c r="L28">
-        <f t="shared" ref="L28:L59" si="60">IFERROR(G28/G29,0)</f>
+        <f t="shared" ref="L28" si="60">IFERROR(G28/G29,0)</f>
         <v>1.1585186678864134</v>
       </c>
       <c r="M28">
-        <f t="shared" ref="M28:M59" si="61">IFERROR(H28/H29, 0)</f>
+        <f t="shared" ref="M28" si="61">IFERROR(H28/H29, 0)</f>
         <v>1.2607810339929204</v>
       </c>
       <c r="N28">
-        <f t="shared" ref="N28:N59" si="62">IFERROR(I28/I29, 0)</f>
+        <f t="shared" ref="N28" si="62">IFERROR(I28/I29, 0)</f>
         <v>1.0804608553856565</v>
       </c>
       <c r="O28">
-        <f t="shared" ref="O28:O59" si="63">IFERROR(J28/J29, 0)</f>
+        <f t="shared" ref="O28" si="63">IFERROR(J28/J29, 0)</f>
         <v>2.1306950745795402E-204</v>
       </c>
       <c r="Q28" t="str">
-        <f t="shared" ref="Q28:Q59" si="64">_xlfn.CONCAT(ROUND(L28, 2), " (", ROUND(N28,2), " - ", ROUND(M28,2),  ")", IF(AND(O28 &lt;0.05, NOT(ISBLANK(O28))), "*", " ") )</f>
+        <f t="shared" ref="Q28" si="64">_xlfn.CONCAT(ROUND(L28, 2), " (", ROUND(N28,2), " - ", ROUND(M28,2),  ")", IF(AND(O28 &lt;0.05, NOT(ISBLANK(O28))), "*", " ") )</f>
         <v>1.16 (1.08 - 1.26)*</v>
       </c>
     </row>
@@ -15759,23 +15758,23 @@
         <v>0</v>
       </c>
       <c r="L30">
-        <f t="shared" ref="L30:L61" si="65">IFERROR(G30/G31,0)</f>
+        <f t="shared" ref="L30" si="65">IFERROR(G30/G31,0)</f>
         <v>0.92536029434536682</v>
       </c>
       <c r="M30">
-        <f t="shared" ref="M30:M61" si="66">IFERROR(H30/H31, 0)</f>
+        <f t="shared" ref="M30" si="66">IFERROR(H30/H31, 0)</f>
         <v>0.94279582994576505</v>
       </c>
       <c r="N30">
-        <f t="shared" ref="N30:N61" si="67">IFERROR(I30/I31, 0)</f>
+        <f t="shared" ref="N30" si="67">IFERROR(I30/I31, 0)</f>
         <v>0.90944808380056863</v>
       </c>
       <c r="O30">
-        <f t="shared" ref="O30:O61" si="68">IFERROR(J30/J31, 0)</f>
+        <f t="shared" ref="O30" si="68">IFERROR(J30/J31, 0)</f>
         <v>0</v>
       </c>
       <c r="Q30" t="str">
-        <f t="shared" ref="Q30:Q61" si="69">_xlfn.CONCAT(ROUND(L30, 2), " (", ROUND(N30,2), " - ", ROUND(M30,2),  ")", IF(AND(O30 &lt;0.05, NOT(ISBLANK(O30))), "*", " ") )</f>
+        <f t="shared" ref="Q30" si="69">_xlfn.CONCAT(ROUND(L30, 2), " (", ROUND(N30,2), " - ", ROUND(M30,2),  ")", IF(AND(O30 &lt;0.05, NOT(ISBLANK(O30))), "*", " ") )</f>
         <v>0.93 (0.91 - 0.94)*</v>
       </c>
     </row>
@@ -15863,23 +15862,23 @@
         <v>1.7245181450306901E-139</v>
       </c>
       <c r="L32">
-        <f t="shared" ref="L32:L63" si="70">IFERROR(G32/G33,0)</f>
+        <f t="shared" ref="L32" si="70">IFERROR(G32/G33,0)</f>
         <v>1.2351218299140501</v>
       </c>
       <c r="M32">
-        <f t="shared" ref="M32:M63" si="71">IFERROR(H32/H33, 0)</f>
+        <f t="shared" ref="M32" si="71">IFERROR(H32/H33, 0)</f>
         <v>1.3521192673768416</v>
       </c>
       <c r="N32">
-        <f t="shared" ref="N32:N63" si="72">IFERROR(I32/I33, 0)</f>
+        <f t="shared" ref="N32" si="72">IFERROR(I32/I33, 0)</f>
         <v>1.1500056010643802</v>
       </c>
       <c r="O32">
-        <f t="shared" ref="O32:O63" si="73">IFERROR(J32/J33, 0)</f>
+        <f t="shared" ref="O32" si="73">IFERROR(J32/J33, 0)</f>
         <v>9.0589328275757676E-105</v>
       </c>
       <c r="Q32" t="str">
-        <f t="shared" ref="Q32:Q63" si="74">_xlfn.CONCAT(ROUND(L32, 2), " (", ROUND(N32,2), " - ", ROUND(M32,2),  ")", IF(AND(O32 &lt;0.05, NOT(ISBLANK(O32))), "*", " ") )</f>
+        <f t="shared" ref="Q32" si="74">_xlfn.CONCAT(ROUND(L32, 2), " (", ROUND(N32,2), " - ", ROUND(M32,2),  ")", IF(AND(O32 &lt;0.05, NOT(ISBLANK(O32))), "*", " ") )</f>
         <v>1.24 (1.15 - 1.35)*</v>
       </c>
     </row>
@@ -15967,23 +15966,23 @@
         <v>0</v>
       </c>
       <c r="L34">
-        <f t="shared" ref="L34:L65" si="75">IFERROR(G34/G35,0)</f>
+        <f t="shared" ref="L34" si="75">IFERROR(G34/G35,0)</f>
         <v>0.95835957729682641</v>
       </c>
       <c r="M34">
-        <f t="shared" ref="M34:M65" si="76">IFERROR(H34/H35, 0)</f>
+        <f t="shared" ref="M34" si="76">IFERROR(H34/H35, 0)</f>
         <v>0.99587478366190563</v>
       </c>
       <c r="N34">
-        <f t="shared" ref="N34:N65" si="77">IFERROR(I34/I35, 0)</f>
+        <f t="shared" ref="N34" si="77">IFERROR(I34/I35, 0)</f>
         <v>0.92685126755739888</v>
       </c>
       <c r="O34">
-        <f t="shared" ref="O34:O65" si="78">IFERROR(J34/J35, 0)</f>
+        <f t="shared" ref="O34" si="78">IFERROR(J34/J35, 0)</f>
         <v>0</v>
       </c>
       <c r="Q34" t="str">
-        <f t="shared" ref="Q34:Q65" si="79">_xlfn.CONCAT(ROUND(L34, 2), " (", ROUND(N34,2), " - ", ROUND(M34,2),  ")", IF(AND(O34 &lt;0.05, NOT(ISBLANK(O34))), "*", " ") )</f>
+        <f t="shared" ref="Q34" si="79">_xlfn.CONCAT(ROUND(L34, 2), " (", ROUND(N34,2), " - ", ROUND(M34,2),  ")", IF(AND(O34 &lt;0.05, NOT(ISBLANK(O34))), "*", " ") )</f>
         <v>0.96 (0.93 - 1)*</v>
       </c>
     </row>
@@ -16071,23 +16070,23 @@
         <v>1.8390630319324302E-42</v>
       </c>
       <c r="L36">
-        <f t="shared" ref="L36:L67" si="80">IFERROR(G36/G37,0)</f>
+        <f t="shared" ref="L36" si="80">IFERROR(G36/G37,0)</f>
         <v>1.3072057205726311</v>
       </c>
       <c r="M36">
-        <f t="shared" ref="M36:M67" si="81">IFERROR(H36/H37, 0)</f>
+        <f t="shared" ref="M36" si="81">IFERROR(H36/H37, 0)</f>
         <v>1.770251869656674</v>
       </c>
       <c r="N36">
-        <f t="shared" ref="N36:N67" si="82">IFERROR(I36/I37, 0)</f>
+        <f t="shared" ref="N36" si="82">IFERROR(I36/I37, 0)</f>
         <v>1.0930595439470863</v>
       </c>
       <c r="O36">
-        <f t="shared" ref="O36:O67" si="83">IFERROR(J36/J37, 0)</f>
+        <f t="shared" ref="O36" si="83">IFERROR(J36/J37, 0)</f>
         <v>1.8990560416017504E-35</v>
       </c>
       <c r="Q36" t="str">
-        <f t="shared" ref="Q36:Q67" si="84">_xlfn.CONCAT(ROUND(L36, 2), " (", ROUND(N36,2), " - ", ROUND(M36,2),  ")", IF(AND(O36 &lt;0.05, NOT(ISBLANK(O36))), "*", " ") )</f>
+        <f t="shared" ref="Q36" si="84">_xlfn.CONCAT(ROUND(L36, 2), " (", ROUND(N36,2), " - ", ROUND(M36,2),  ")", IF(AND(O36 &lt;0.05, NOT(ISBLANK(O36))), "*", " ") )</f>
         <v>1.31 (1.09 - 1.77)*</v>
       </c>
     </row>
@@ -16175,23 +16174,23 @@
         <v>1.07160073247481E-41</v>
       </c>
       <c r="L38">
-        <f t="shared" ref="L38:L69" si="85">IFERROR(G38/G39,0)</f>
+        <f t="shared" ref="L38" si="85">IFERROR(G38/G39,0)</f>
         <v>1.099999999969645</v>
       </c>
       <c r="M38">
-        <f t="shared" ref="M38:M69" si="86">IFERROR(H38/H39, 0)</f>
+        <f t="shared" ref="M38" si="86">IFERROR(H38/H39, 0)</f>
         <v>1.3635803690510457</v>
       </c>
       <c r="N38">
-        <f t="shared" ref="N38:N69" si="87">IFERROR(I38/I39, 0)</f>
+        <f t="shared" ref="N38" si="87">IFERROR(I38/I39, 0)</f>
         <v>1</v>
       </c>
       <c r="O38">
-        <f t="shared" ref="O38:O69" si="88">IFERROR(J38/J39, 0)</f>
+        <f t="shared" ref="O38" si="88">IFERROR(J38/J39, 0)</f>
         <v>4.0661228295695771E-32</v>
       </c>
       <c r="Q38" t="str">
-        <f t="shared" ref="Q38:Q69" si="89">_xlfn.CONCAT(ROUND(L38, 2), " (", ROUND(N38,2), " - ", ROUND(M38,2),  ")", IF(AND(O38 &lt;0.05, NOT(ISBLANK(O38))), "*", " ") )</f>
+        <f t="shared" ref="Q38" si="89">_xlfn.CONCAT(ROUND(L38, 2), " (", ROUND(N38,2), " - ", ROUND(M38,2),  ")", IF(AND(O38 &lt;0.05, NOT(ISBLANK(O38))), "*", " ") )</f>
         <v>1.1 (1 - 1.36)*</v>
       </c>
     </row>
@@ -16279,23 +16278,23 @@
         <v>0</v>
       </c>
       <c r="L40">
-        <f t="shared" ref="L40:L71" si="90">IFERROR(G40/G41,0)</f>
+        <f t="shared" ref="L40" si="90">IFERROR(G40/G41,0)</f>
         <v>1.0000002402974009</v>
       </c>
       <c r="M40">
-        <f t="shared" ref="M40:M71" si="91">IFERROR(H40/H41, 0)</f>
+        <f t="shared" ref="M40" si="91">IFERROR(H40/H41, 0)</f>
         <v>0</v>
       </c>
       <c r="N40">
-        <f t="shared" ref="N40:N71" si="92">IFERROR(I40/I41, 0)</f>
+        <f t="shared" ref="N40" si="92">IFERROR(I40/I41, 0)</f>
         <v>1</v>
       </c>
       <c r="O40">
-        <f t="shared" ref="O40:O71" si="93">IFERROR(J40/J41, 0)</f>
+        <f t="shared" ref="O40" si="93">IFERROR(J40/J41, 0)</f>
         <v>0</v>
       </c>
       <c r="Q40" t="str">
-        <f t="shared" ref="Q40:Q71" si="94">_xlfn.CONCAT(ROUND(L40, 2), " (", ROUND(N40,2), " - ", ROUND(M40,2),  ")", IF(AND(O40 &lt;0.05, NOT(ISBLANK(O40))), "*", " ") )</f>
+        <f t="shared" ref="Q40" si="94">_xlfn.CONCAT(ROUND(L40, 2), " (", ROUND(N40,2), " - ", ROUND(M40,2),  ")", IF(AND(O40 &lt;0.05, NOT(ISBLANK(O40))), "*", " ") )</f>
         <v>1 (1 - 0)*</v>
       </c>
     </row>
@@ -16383,23 +16382,23 @@
         <v>0</v>
       </c>
       <c r="L42">
-        <f t="shared" ref="L42:L73" si="95">IFERROR(G42/G43,0)</f>
+        <f t="shared" ref="L42" si="95">IFERROR(G42/G43,0)</f>
         <v>1.0322158116321629</v>
       </c>
       <c r="M42">
-        <f t="shared" ref="M42:M73" si="96">IFERROR(H42/H43, 0)</f>
+        <f t="shared" ref="M42" si="96">IFERROR(H42/H43, 0)</f>
         <v>1.049438161328645</v>
       </c>
       <c r="N42">
-        <f t="shared" ref="N42:N73" si="97">IFERROR(I42/I43, 0)</f>
+        <f t="shared" ref="N42" si="97">IFERROR(I42/I43, 0)</f>
         <v>1.0165295582937688</v>
       </c>
       <c r="O42">
-        <f t="shared" ref="O42:O73" si="98">IFERROR(J42/J43, 0)</f>
+        <f t="shared" ref="O42" si="98">IFERROR(J42/J43, 0)</f>
         <v>0</v>
       </c>
       <c r="Q42" t="str">
-        <f t="shared" ref="Q42:Q73" si="99">_xlfn.CONCAT(ROUND(L42, 2), " (", ROUND(N42,2), " - ", ROUND(M42,2),  ")", IF(AND(O42 &lt;0.05, NOT(ISBLANK(O42))), "*", " ") )</f>
+        <f t="shared" ref="Q42" si="99">_xlfn.CONCAT(ROUND(L42, 2), " (", ROUND(N42,2), " - ", ROUND(M42,2),  ")", IF(AND(O42 &lt;0.05, NOT(ISBLANK(O42))), "*", " ") )</f>
         <v>1.03 (1.02 - 1.05)*</v>
       </c>
     </row>
@@ -16487,23 +16486,23 @@
         <v>8.2880721088018199E-196</v>
       </c>
       <c r="L44">
-        <f t="shared" ref="L44:L75" si="100">IFERROR(G44/G45,0)</f>
+        <f t="shared" ref="L44" si="100">IFERROR(G44/G45,0)</f>
         <v>1.2734734003476409</v>
       </c>
       <c r="M44">
-        <f t="shared" ref="M44:M75" si="101">IFERROR(H44/H45, 0)</f>
+        <f t="shared" ref="M44" si="101">IFERROR(H44/H45, 0)</f>
         <v>1.3605099392037572</v>
       </c>
       <c r="N44">
-        <f t="shared" ref="N44:N75" si="102">IFERROR(I44/I45, 0)</f>
+        <f t="shared" ref="N44" si="102">IFERROR(I44/I45, 0)</f>
         <v>1.205837353399388</v>
       </c>
       <c r="O44">
-        <f t="shared" ref="O44:O75" si="103">IFERROR(J44/J45, 0)</f>
+        <f t="shared" ref="O44" si="103">IFERROR(J44/J45, 0)</f>
         <v>1.7123236815032867E-141</v>
       </c>
       <c r="Q44" t="str">
-        <f t="shared" ref="Q44:Q75" si="104">_xlfn.CONCAT(ROUND(L44, 2), " (", ROUND(N44,2), " - ", ROUND(M44,2),  ")", IF(AND(O44 &lt;0.05, NOT(ISBLANK(O44))), "*", " ") )</f>
+        <f t="shared" ref="Q44" si="104">_xlfn.CONCAT(ROUND(L44, 2), " (", ROUND(N44,2), " - ", ROUND(M44,2),  ")", IF(AND(O44 &lt;0.05, NOT(ISBLANK(O44))), "*", " ") )</f>
         <v>1.27 (1.21 - 1.36)*</v>
       </c>
     </row>
@@ -16591,23 +16590,23 @@
         <v>3.9027411100951802E-82</v>
       </c>
       <c r="L46">
-        <f t="shared" ref="L46:L77" si="105">IFERROR(G46/G47,0)</f>
+        <f t="shared" ref="L46" si="105">IFERROR(G46/G47,0)</f>
         <v>1.026941685765224</v>
       </c>
       <c r="M46">
-        <f t="shared" ref="M46:M77" si="106">IFERROR(H46/H47, 0)</f>
+        <f t="shared" ref="M46" si="106">IFERROR(H46/H47, 0)</f>
         <v>1.0656286980069842</v>
       </c>
       <c r="N46">
-        <f t="shared" ref="N46:N77" si="107">IFERROR(I46/I47, 0)</f>
+        <f t="shared" ref="N46" si="107">IFERROR(I46/I47, 0)</f>
         <v>0.99743936649098641</v>
       </c>
       <c r="O46">
-        <f t="shared" ref="O46:O77" si="108">IFERROR(J46/J47, 0)</f>
+        <f t="shared" ref="O46" si="108">IFERROR(J46/J47, 0)</f>
         <v>6.8042557323835812E-35</v>
       </c>
       <c r="Q46" t="str">
-        <f t="shared" ref="Q46:Q77" si="109">_xlfn.CONCAT(ROUND(L46, 2), " (", ROUND(N46,2), " - ", ROUND(M46,2),  ")", IF(AND(O46 &lt;0.05, NOT(ISBLANK(O46))), "*", " ") )</f>
+        <f t="shared" ref="Q46" si="109">_xlfn.CONCAT(ROUND(L46, 2), " (", ROUND(N46,2), " - ", ROUND(M46,2),  ")", IF(AND(O46 &lt;0.05, NOT(ISBLANK(O46))), "*", " ") )</f>
         <v>1.03 (1 - 1.07)*</v>
       </c>
     </row>
@@ -16695,23 +16694,23 @@
         <v>2.8208218528763002E-41</v>
       </c>
       <c r="L48">
-        <f t="shared" ref="L48:L79" si="110">IFERROR(G48/G49,0)</f>
+        <f t="shared" ref="L48" si="110">IFERROR(G48/G49,0)</f>
         <v>1.4599785444683031</v>
       </c>
       <c r="M48">
-        <f t="shared" ref="M48:M79" si="111">IFERROR(H48/H49, 0)</f>
+        <f t="shared" ref="M48" si="111">IFERROR(H48/H49, 0)</f>
         <v>1.7837736079602442</v>
       </c>
       <c r="N48">
-        <f t="shared" ref="N48:N79" si="112">IFERROR(I48/I49, 0)</f>
+        <f t="shared" ref="N48" si="112">IFERROR(I48/I49, 0)</f>
         <v>1.2859090517476126</v>
       </c>
       <c r="O48">
-        <f t="shared" ref="O48:O79" si="113">IFERROR(J48/J49, 0)</f>
+        <f t="shared" ref="O48" si="113">IFERROR(J48/J49, 0)</f>
         <v>3.9388370316726923E-31</v>
       </c>
       <c r="Q48" t="str">
-        <f t="shared" ref="Q48:Q79" si="114">_xlfn.CONCAT(ROUND(L48, 2), " (", ROUND(N48,2), " - ", ROUND(M48,2),  ")", IF(AND(O48 &lt;0.05, NOT(ISBLANK(O48))), "*", " ") )</f>
+        <f t="shared" ref="Q48" si="114">_xlfn.CONCAT(ROUND(L48, 2), " (", ROUND(N48,2), " - ", ROUND(M48,2),  ")", IF(AND(O48 &lt;0.05, NOT(ISBLANK(O48))), "*", " ") )</f>
         <v>1.46 (1.29 - 1.78)*</v>
       </c>
     </row>
@@ -16799,23 +16798,23 @@
         <v>0</v>
       </c>
       <c r="L50">
-        <f t="shared" ref="L50:L81" si="115">IFERROR(G50/G51,0)</f>
+        <f t="shared" ref="L50" si="115">IFERROR(G50/G51,0)</f>
         <v>1.0629573212192529</v>
       </c>
       <c r="M50">
-        <f t="shared" ref="M50:M81" si="116">IFERROR(H50/H51, 0)</f>
+        <f t="shared" ref="M50" si="116">IFERROR(H50/H51, 0)</f>
         <v>1.0865511965874297</v>
       </c>
       <c r="N50">
-        <f t="shared" ref="N50:N81" si="117">IFERROR(I50/I51, 0)</f>
+        <f t="shared" ref="N50" si="117">IFERROR(I50/I51, 0)</f>
         <v>1.042289534802328</v>
       </c>
       <c r="O50">
-        <f t="shared" ref="O50:O81" si="118">IFERROR(J50/J51, 0)</f>
+        <f t="shared" ref="O50" si="118">IFERROR(J50/J51, 0)</f>
         <v>0</v>
       </c>
       <c r="Q50" t="str">
-        <f t="shared" ref="Q50:Q81" si="119">_xlfn.CONCAT(ROUND(L50, 2), " (", ROUND(N50,2), " - ", ROUND(M50,2),  ")", IF(AND(O50 &lt;0.05, NOT(ISBLANK(O50))), "*", " ") )</f>
+        <f t="shared" ref="Q50" si="119">_xlfn.CONCAT(ROUND(L50, 2), " (", ROUND(N50,2), " - ", ROUND(M50,2),  ")", IF(AND(O50 &lt;0.05, NOT(ISBLANK(O50))), "*", " ") )</f>
         <v>1.06 (1.04 - 1.09)*</v>
       </c>
     </row>
@@ -16903,23 +16902,23 @@
         <v>3.0941930923561102E-82</v>
       </c>
       <c r="L52">
-        <f t="shared" ref="L52:L83" si="120">IFERROR(G52/G53,0)</f>
+        <f t="shared" ref="L52" si="120">IFERROR(G52/G53,0)</f>
         <v>1.198250728864753</v>
       </c>
       <c r="M52">
-        <f t="shared" ref="M52:M83" si="121">IFERROR(H52/H53, 0)</f>
+        <f t="shared" ref="M52" si="121">IFERROR(H52/H53, 0)</f>
         <v>1.3049185986517602</v>
       </c>
       <c r="N52">
-        <f t="shared" ref="N52:N83" si="122">IFERROR(I52/I53, 0)</f>
+        <f t="shared" ref="N52" si="122">IFERROR(I52/I53, 0)</f>
         <v>1.1234233934540225</v>
       </c>
       <c r="O52">
-        <f t="shared" ref="O52:O83" si="123">IFERROR(J52/J53, 0)</f>
+        <f t="shared" ref="O52" si="123">IFERROR(J52/J53, 0)</f>
         <v>5.5376340334540013E-54</v>
       </c>
       <c r="Q52" t="str">
-        <f t="shared" ref="Q52:Q83" si="124">_xlfn.CONCAT(ROUND(L52, 2), " (", ROUND(N52,2), " - ", ROUND(M52,2),  ")", IF(AND(O52 &lt;0.05, NOT(ISBLANK(O52))), "*", " ") )</f>
+        <f t="shared" ref="Q52" si="124">_xlfn.CONCAT(ROUND(L52, 2), " (", ROUND(N52,2), " - ", ROUND(M52,2),  ")", IF(AND(O52 &lt;0.05, NOT(ISBLANK(O52))), "*", " ") )</f>
         <v>1.2 (1.12 - 1.3)*</v>
       </c>
     </row>
@@ -17007,23 +17006,23 @@
         <v>4.0980857948529698E-289</v>
       </c>
       <c r="L54">
-        <f t="shared" ref="L54:L85" si="125">IFERROR(G54/G55,0)</f>
+        <f t="shared" ref="L54" si="125">IFERROR(G54/G55,0)</f>
         <v>0.96119402985107494</v>
       </c>
       <c r="M54">
-        <f t="shared" ref="M54:M85" si="126">IFERROR(H54/H55, 0)</f>
+        <f t="shared" ref="M54" si="126">IFERROR(H54/H55, 0)</f>
         <v>0.99291587271291815</v>
       </c>
       <c r="N54">
-        <f t="shared" ref="N54:N85" si="127">IFERROR(I54/I55, 0)</f>
+        <f t="shared" ref="N54" si="127">IFERROR(I54/I55, 0)</f>
         <v>0.93439725047205591</v>
       </c>
       <c r="O54">
-        <f t="shared" ref="O54:O85" si="128">IFERROR(J54/J55, 0)</f>
+        <f t="shared" ref="O54" si="128">IFERROR(J54/J55, 0)</f>
         <v>6.970081641867964E-170</v>
       </c>
       <c r="Q54" t="str">
-        <f t="shared" ref="Q54:Q85" si="129">_xlfn.CONCAT(ROUND(L54, 2), " (", ROUND(N54,2), " - ", ROUND(M54,2),  ")", IF(AND(O54 &lt;0.05, NOT(ISBLANK(O54))), "*", " ") )</f>
+        <f t="shared" ref="Q54" si="129">_xlfn.CONCAT(ROUND(L54, 2), " (", ROUND(N54,2), " - ", ROUND(M54,2),  ")", IF(AND(O54 &lt;0.05, NOT(ISBLANK(O54))), "*", " ") )</f>
         <v>0.96 (0.93 - 0.99)*</v>
       </c>
     </row>
@@ -17111,23 +17110,23 @@
         <v>2.1169174738636902E-73</v>
       </c>
       <c r="L56">
-        <f t="shared" ref="L56:L87" si="130">IFERROR(G56/G57,0)</f>
+        <f t="shared" ref="L56" si="130">IFERROR(G56/G57,0)</f>
         <v>1.1462785564570992</v>
       </c>
       <c r="M56">
-        <f t="shared" ref="M56:M87" si="131">IFERROR(H56/H57, 0)</f>
+        <f t="shared" ref="M56" si="131">IFERROR(H56/H57, 0)</f>
         <v>1.3214928584224741</v>
       </c>
       <c r="N56">
-        <f t="shared" ref="N56:N87" si="132">IFERROR(I56/I57, 0)</f>
+        <f t="shared" ref="N56" si="132">IFERROR(I56/I57, 0)</f>
         <v>1.0357551128668727</v>
       </c>
       <c r="O56">
-        <f t="shared" ref="O56:O87" si="133">IFERROR(J56/J57, 0)</f>
+        <f t="shared" ref="O56" si="133">IFERROR(J56/J57, 0)</f>
         <v>4.3748093231211315E-56</v>
       </c>
       <c r="Q56" t="str">
-        <f t="shared" ref="Q56:Q87" si="134">_xlfn.CONCAT(ROUND(L56, 2), " (", ROUND(N56,2), " - ", ROUND(M56,2),  ")", IF(AND(O56 &lt;0.05, NOT(ISBLANK(O56))), "*", " ") )</f>
+        <f t="shared" ref="Q56" si="134">_xlfn.CONCAT(ROUND(L56, 2), " (", ROUND(N56,2), " - ", ROUND(M56,2),  ")", IF(AND(O56 &lt;0.05, NOT(ISBLANK(O56))), "*", " ") )</f>
         <v>1.15 (1.04 - 1.32)*</v>
       </c>
     </row>
@@ -17215,23 +17214,23 @@
         <v>2.7820948046816102E-122</v>
       </c>
       <c r="L58">
-        <f t="shared" ref="L58:L89" si="135">IFERROR(G58/G59,0)</f>
+        <f t="shared" ref="L58" si="135">IFERROR(G58/G59,0)</f>
         <v>1.0557951017587985</v>
       </c>
       <c r="M58">
-        <f t="shared" ref="M58:M89" si="136">IFERROR(H58/H59, 0)</f>
+        <f t="shared" ref="M58" si="136">IFERROR(H58/H59, 0)</f>
         <v>1.1453408118450696</v>
       </c>
       <c r="N58">
-        <f t="shared" ref="N58:N89" si="137">IFERROR(I58/I59, 0)</f>
+        <f t="shared" ref="N58" si="137">IFERROR(I58/I59, 0)</f>
         <v>0.99028485714820214</v>
       </c>
       <c r="O58">
-        <f t="shared" ref="O58:O89" si="138">IFERROR(J58/J59, 0)</f>
+        <f t="shared" ref="O58" si="138">IFERROR(J58/J59, 0)</f>
         <v>2.3035786174036447E-86</v>
       </c>
       <c r="Q58" t="str">
-        <f t="shared" ref="Q58:Q89" si="139">_xlfn.CONCAT(ROUND(L58, 2), " (", ROUND(N58,2), " - ", ROUND(M58,2),  ")", IF(AND(O58 &lt;0.05, NOT(ISBLANK(O58))), "*", " ") )</f>
+        <f t="shared" ref="Q58" si="139">_xlfn.CONCAT(ROUND(L58, 2), " (", ROUND(N58,2), " - ", ROUND(M58,2),  ")", IF(AND(O58 &lt;0.05, NOT(ISBLANK(O58))), "*", " ") )</f>
         <v>1.06 (0.99 - 1.15)*</v>
       </c>
     </row>
@@ -17319,23 +17318,23 @@
         <v>7.3429598082326996E-25</v>
       </c>
       <c r="L60">
-        <f t="shared" ref="L60:L91" si="140">IFERROR(G60/G61,0)</f>
+        <f t="shared" ref="L60" si="140">IFERROR(G60/G61,0)</f>
         <v>0.93749999999940259</v>
       </c>
       <c r="M60">
-        <f t="shared" ref="M60:M91" si="141">IFERROR(H60/H61, 0)</f>
+        <f t="shared" ref="M60" si="141">IFERROR(H60/H61, 0)</f>
         <v>1.1840488957407367</v>
       </c>
       <c r="N60">
-        <f t="shared" ref="N60:N91" si="142">IFERROR(I60/I61, 0)</f>
+        <f t="shared" ref="N60" si="142">IFERROR(I60/I61, 0)</f>
         <v>0.82119642184562514</v>
       </c>
       <c r="O60">
-        <f t="shared" ref="O60:O91" si="143">IFERROR(J60/J61, 0)</f>
+        <f t="shared" ref="O60" si="143">IFERROR(J60/J61, 0)</f>
         <v>1.544762222307857E-17</v>
       </c>
       <c r="Q60" t="str">
-        <f t="shared" ref="Q60:Q91" si="144">_xlfn.CONCAT(ROUND(L60, 2), " (", ROUND(N60,2), " - ", ROUND(M60,2),  ")", IF(AND(O60 &lt;0.05, NOT(ISBLANK(O60))), "*", " ") )</f>
+        <f t="shared" ref="Q60" si="144">_xlfn.CONCAT(ROUND(L60, 2), " (", ROUND(N60,2), " - ", ROUND(M60,2),  ")", IF(AND(O60 &lt;0.05, NOT(ISBLANK(O60))), "*", " ") )</f>
         <v>0.94 (0.82 - 1.18)*</v>
       </c>
     </row>
@@ -17423,23 +17422,23 @@
         <v>0</v>
       </c>
       <c r="L62">
-        <f t="shared" ref="L62:L93" si="145">IFERROR(G62/G63,0)</f>
+        <f t="shared" ref="L62" si="145">IFERROR(G62/G63,0)</f>
         <v>0.92177924328403849</v>
       </c>
       <c r="M62">
-        <f t="shared" ref="M62:M93" si="146">IFERROR(H62/H63, 0)</f>
+        <f t="shared" ref="M62" si="146">IFERROR(H62/H63, 0)</f>
         <v>0.93525479936324085</v>
       </c>
       <c r="N62">
-        <f t="shared" ref="N62:N93" si="147">IFERROR(I62/I63, 0)</f>
+        <f t="shared" ref="N62" si="147">IFERROR(I62/I63, 0)</f>
         <v>0.90908137453988014</v>
       </c>
       <c r="O62">
-        <f t="shared" ref="O62:O93" si="148">IFERROR(J62/J63, 0)</f>
+        <f t="shared" ref="O62" si="148">IFERROR(J62/J63, 0)</f>
         <v>0</v>
       </c>
       <c r="Q62" t="str">
-        <f t="shared" ref="Q62:Q93" si="149">_xlfn.CONCAT(ROUND(L62, 2), " (", ROUND(N62,2), " - ", ROUND(M62,2),  ")", IF(AND(O62 &lt;0.05, NOT(ISBLANK(O62))), "*", " ") )</f>
+        <f t="shared" ref="Q62" si="149">_xlfn.CONCAT(ROUND(L62, 2), " (", ROUND(N62,2), " - ", ROUND(M62,2),  ")", IF(AND(O62 &lt;0.05, NOT(ISBLANK(O62))), "*", " ") )</f>
         <v>0.92 (0.91 - 0.94)*</v>
       </c>
     </row>
@@ -17527,23 +17526,23 @@
         <v>0</v>
       </c>
       <c r="L64">
-        <f t="shared" ref="L64:L95" si="150">IFERROR(G64/G65,0)</f>
+        <f t="shared" ref="L64" si="150">IFERROR(G64/G65,0)</f>
         <v>1.0248255859873261</v>
       </c>
       <c r="M64">
-        <f t="shared" ref="M64:M95" si="151">IFERROR(H64/H65, 0)</f>
+        <f t="shared" ref="M64" si="151">IFERROR(H64/H65, 0)</f>
         <v>1.0589279032683525</v>
       </c>
       <c r="N64">
-        <f t="shared" ref="N64:N95" si="152">IFERROR(I64/I65, 0)</f>
+        <f t="shared" ref="N64" si="152">IFERROR(I64/I65, 0)</f>
         <v>0.9945006203970127</v>
       </c>
       <c r="O64">
-        <f t="shared" ref="O64:O95" si="153">IFERROR(J64/J65, 0)</f>
+        <f t="shared" ref="O64" si="153">IFERROR(J64/J65, 0)</f>
         <v>0</v>
       </c>
       <c r="Q64" t="str">
-        <f t="shared" ref="Q64:Q95" si="154">_xlfn.CONCAT(ROUND(L64, 2), " (", ROUND(N64,2), " - ", ROUND(M64,2),  ")", IF(AND(O64 &lt;0.05, NOT(ISBLANK(O64))), "*", " ") )</f>
+        <f t="shared" ref="Q64" si="154">_xlfn.CONCAT(ROUND(L64, 2), " (", ROUND(N64,2), " - ", ROUND(M64,2),  ")", IF(AND(O64 &lt;0.05, NOT(ISBLANK(O64))), "*", " ") )</f>
         <v>1.02 (0.99 - 1.06)*</v>
       </c>
     </row>
@@ -17631,23 +17630,23 @@
         <v>0</v>
       </c>
       <c r="L66">
-        <f t="shared" ref="L66:L97" si="155">IFERROR(G66/G67,0)</f>
+        <f t="shared" ref="L66" si="155">IFERROR(G66/G67,0)</f>
         <v>0.93439844254720539</v>
       </c>
       <c r="M66">
-        <f t="shared" ref="M66:M97" si="156">IFERROR(H66/H67, 0)</f>
+        <f t="shared" ref="M66" si="156">IFERROR(H66/H67, 0)</f>
         <v>0.95819996078842606</v>
       </c>
       <c r="N66">
-        <f t="shared" ref="N66:N97" si="157">IFERROR(I66/I67, 0)</f>
+        <f t="shared" ref="N66" si="157">IFERROR(I66/I67, 0)</f>
         <v>0.91280784693580808</v>
       </c>
       <c r="O66">
-        <f t="shared" ref="O66:O97" si="158">IFERROR(J66/J67, 0)</f>
+        <f t="shared" ref="O66" si="158">IFERROR(J66/J67, 0)</f>
         <v>0</v>
       </c>
       <c r="Q66" t="str">
-        <f t="shared" ref="Q66:Q97" si="159">_xlfn.CONCAT(ROUND(L66, 2), " (", ROUND(N66,2), " - ", ROUND(M66,2),  ")", IF(AND(O66 &lt;0.05, NOT(ISBLANK(O66))), "*", " ") )</f>
+        <f t="shared" ref="Q66" si="159">_xlfn.CONCAT(ROUND(L66, 2), " (", ROUND(N66,2), " - ", ROUND(M66,2),  ")", IF(AND(O66 &lt;0.05, NOT(ISBLANK(O66))), "*", " ") )</f>
         <v>0.93 (0.91 - 0.96)*</v>
       </c>
     </row>
@@ -17735,23 +17734,23 @@
         <v>0</v>
       </c>
       <c r="L68">
-        <f t="shared" ref="L68:L99" si="160">IFERROR(G68/G69,0)</f>
+        <f t="shared" ref="L68" si="160">IFERROR(G68/G69,0)</f>
         <v>1.0761460678154944</v>
       </c>
       <c r="M68">
-        <f t="shared" ref="M68:M99" si="161">IFERROR(H68/H69, 0)</f>
+        <f t="shared" ref="M68" si="161">IFERROR(H68/H69, 0)</f>
         <v>1.136147129708754</v>
       </c>
       <c r="N68">
-        <f t="shared" ref="N68:N99" si="162">IFERROR(I68/I69, 0)</f>
+        <f t="shared" ref="N68" si="162">IFERROR(I68/I69, 0)</f>
         <v>1.0261654116398404</v>
       </c>
       <c r="O68">
-        <f t="shared" ref="O68:O99" si="163">IFERROR(J68/J69, 0)</f>
+        <f t="shared" ref="O68" si="163">IFERROR(J68/J69, 0)</f>
         <v>0</v>
       </c>
       <c r="Q68" t="str">
-        <f t="shared" ref="Q68:Q99" si="164">_xlfn.CONCAT(ROUND(L68, 2), " (", ROUND(N68,2), " - ", ROUND(M68,2),  ")", IF(AND(O68 &lt;0.05, NOT(ISBLANK(O68))), "*", " ") )</f>
+        <f t="shared" ref="Q68" si="164">_xlfn.CONCAT(ROUND(L68, 2), " (", ROUND(N68,2), " - ", ROUND(M68,2),  ")", IF(AND(O68 &lt;0.05, NOT(ISBLANK(O68))), "*", " ") )</f>
         <v>1.08 (1.03 - 1.14)*</v>
       </c>
     </row>
@@ -17839,23 +17838,23 @@
         <v>0</v>
       </c>
       <c r="L70">
-        <f t="shared" ref="L70:L101" si="165">IFERROR(G70/G71,0)</f>
+        <f t="shared" ref="L70" si="165">IFERROR(G70/G71,0)</f>
         <v>0.89717431869998443</v>
       </c>
       <c r="M70">
-        <f t="shared" ref="M70:M101" si="166">IFERROR(H70/H71, 0)</f>
+        <f t="shared" ref="M70" si="166">IFERROR(H70/H71, 0)</f>
         <v>0.9159515128586988</v>
       </c>
       <c r="N70">
-        <f t="shared" ref="N70:N101" si="167">IFERROR(I70/I71, 0)</f>
+        <f t="shared" ref="N70" si="167">IFERROR(I70/I71, 0)</f>
         <v>0.87997107976259259</v>
       </c>
       <c r="O70">
-        <f t="shared" ref="O70:O101" si="168">IFERROR(J70/J71, 0)</f>
+        <f t="shared" ref="O70" si="168">IFERROR(J70/J71, 0)</f>
         <v>0</v>
       </c>
       <c r="Q70" t="str">
-        <f t="shared" ref="Q70:Q101" si="169">_xlfn.CONCAT(ROUND(L70, 2), " (", ROUND(N70,2), " - ", ROUND(M70,2),  ")", IF(AND(O70 &lt;0.05, NOT(ISBLANK(O70))), "*", " ") )</f>
+        <f t="shared" ref="Q70" si="169">_xlfn.CONCAT(ROUND(L70, 2), " (", ROUND(N70,2), " - ", ROUND(M70,2),  ")", IF(AND(O70 &lt;0.05, NOT(ISBLANK(O70))), "*", " ") )</f>
         <v>0.9 (0.88 - 0.92)*</v>
       </c>
     </row>
@@ -17943,23 +17942,23 @@
         <v>0</v>
       </c>
       <c r="L72">
-        <f t="shared" ref="L72:L103" si="170">IFERROR(G72/G73,0)</f>
+        <f t="shared" ref="L72" si="170">IFERROR(G72/G73,0)</f>
         <v>1.0874773983286028</v>
       </c>
       <c r="M72">
-        <f t="shared" ref="M72:M103" si="171">IFERROR(H72/H73, 0)</f>
+        <f t="shared" ref="M72" si="171">IFERROR(H72/H73, 0)</f>
         <v>1.1441826800033177</v>
       </c>
       <c r="N72">
-        <f t="shared" ref="N72:N103" si="172">IFERROR(I72/I73, 0)</f>
+        <f t="shared" ref="N72" si="172">IFERROR(I72/I73, 0)</f>
         <v>1.0401034467307779</v>
       </c>
       <c r="O72">
-        <f t="shared" ref="O72:O103" si="173">IFERROR(J72/J73, 0)</f>
+        <f t="shared" ref="O72" si="173">IFERROR(J72/J73, 0)</f>
         <v>0</v>
       </c>
       <c r="Q72" t="str">
-        <f t="shared" ref="Q72:Q103" si="174">_xlfn.CONCAT(ROUND(L72, 2), " (", ROUND(N72,2), " - ", ROUND(M72,2),  ")", IF(AND(O72 &lt;0.05, NOT(ISBLANK(O72))), "*", " ") )</f>
+        <f t="shared" ref="Q72" si="174">_xlfn.CONCAT(ROUND(L72, 2), " (", ROUND(N72,2), " - ", ROUND(M72,2),  ")", IF(AND(O72 &lt;0.05, NOT(ISBLANK(O72))), "*", " ") )</f>
         <v>1.09 (1.04 - 1.14)*</v>
       </c>
     </row>
@@ -18047,23 +18046,23 @@
         <v>0</v>
       </c>
       <c r="L74">
-        <f t="shared" ref="L74:L121" si="175">IFERROR(G74/G75,0)</f>
+        <f t="shared" ref="L74" si="175">IFERROR(G74/G75,0)</f>
         <v>1.0258512382615368</v>
       </c>
       <c r="M74">
-        <f t="shared" ref="M74:M120" si="176">IFERROR(H74/H75, 0)</f>
+        <f t="shared" ref="M74" si="176">IFERROR(H74/H75, 0)</f>
         <v>1.0627169760214794</v>
       </c>
       <c r="N74">
-        <f t="shared" ref="N74:N120" si="177">IFERROR(I74/I75, 0)</f>
+        <f t="shared" ref="N74" si="177">IFERROR(I74/I75, 0)</f>
         <v>0.99364255586587502</v>
       </c>
       <c r="O74">
-        <f t="shared" ref="O74:O120" si="178">IFERROR(J74/J75, 0)</f>
+        <f t="shared" ref="O74" si="178">IFERROR(J74/J75, 0)</f>
         <v>0</v>
       </c>
       <c r="Q74" t="str">
-        <f t="shared" ref="Q74:Q120" si="179">_xlfn.CONCAT(ROUND(L74, 2), " (", ROUND(N74,2), " - ", ROUND(M74,2),  ")", IF(AND(O74 &lt;0.05, NOT(ISBLANK(O74))), "*", " ") )</f>
+        <f t="shared" ref="Q74" si="179">_xlfn.CONCAT(ROUND(L74, 2), " (", ROUND(N74,2), " - ", ROUND(M74,2),  ")", IF(AND(O74 &lt;0.05, NOT(ISBLANK(O74))), "*", " ") )</f>
         <v>1.03 (0.99 - 1.06)*</v>
       </c>
     </row>
@@ -18151,23 +18150,23 @@
         <v>7.2943952030367593E-251</v>
       </c>
       <c r="L76">
-        <f t="shared" ref="L76:L121" si="180">IFERROR(G76/G77,0)</f>
+        <f t="shared" ref="L76" si="180">IFERROR(G76/G77,0)</f>
         <v>0.92314060111927043</v>
       </c>
       <c r="M76">
-        <f t="shared" ref="M76:M120" si="181">IFERROR(H76/H77, 0)</f>
+        <f t="shared" ref="M76" si="181">IFERROR(H76/H77, 0)</f>
         <v>0.97157781228591689</v>
       </c>
       <c r="N76">
-        <f t="shared" ref="N76:N120" si="182">IFERROR(I76/I77, 0)</f>
+        <f t="shared" ref="N76" si="182">IFERROR(I76/I77, 0)</f>
         <v>0.88390091668631821</v>
       </c>
       <c r="O76">
-        <f t="shared" ref="O76:O120" si="183">IFERROR(J76/J77, 0)</f>
+        <f t="shared" ref="O76" si="183">IFERROR(J76/J77, 0)</f>
         <v>1.084939084261182E-173</v>
       </c>
       <c r="Q76" t="str">
-        <f t="shared" ref="Q76:Q120" si="184">_xlfn.CONCAT(ROUND(L76, 2), " (", ROUND(N76,2), " - ", ROUND(M76,2),  ")", IF(AND(O76 &lt;0.05, NOT(ISBLANK(O76))), "*", " ") )</f>
+        <f t="shared" ref="Q76" si="184">_xlfn.CONCAT(ROUND(L76, 2), " (", ROUND(N76,2), " - ", ROUND(M76,2),  ")", IF(AND(O76 &lt;0.05, NOT(ISBLANK(O76))), "*", " ") )</f>
         <v>0.92 (0.88 - 0.97)*</v>
       </c>
     </row>
@@ -18255,23 +18254,23 @@
         <v>1.4301001472263699E-172</v>
       </c>
       <c r="L78">
-        <f t="shared" ref="L78:L121" si="185">IFERROR(G78/G79,0)</f>
+        <f t="shared" ref="L78" si="185">IFERROR(G78/G79,0)</f>
         <v>1.0146315789477189</v>
       </c>
       <c r="M78">
-        <f t="shared" ref="M78:M120" si="186">IFERROR(H78/H79, 0)</f>
+        <f t="shared" ref="M78" si="186">IFERROR(H78/H79, 0)</f>
         <v>1.0796881736601824</v>
       </c>
       <c r="N78">
-        <f t="shared" ref="N78:N120" si="187">IFERROR(I78/I79, 0)</f>
+        <f t="shared" ref="N78" si="187">IFERROR(I78/I79, 0)</f>
         <v>0.96413730912602147</v>
       </c>
       <c r="O78">
-        <f t="shared" ref="O78:O120" si="188">IFERROR(J78/J79, 0)</f>
+        <f t="shared" ref="O78" si="188">IFERROR(J78/J79, 0)</f>
         <v>9.2959534633768579E-119</v>
       </c>
       <c r="Q78" t="str">
-        <f t="shared" ref="Q78:Q120" si="189">_xlfn.CONCAT(ROUND(L78, 2), " (", ROUND(N78,2), " - ", ROUND(M78,2),  ")", IF(AND(O78 &lt;0.05, NOT(ISBLANK(O78))), "*", " ") )</f>
+        <f t="shared" ref="Q78" si="189">_xlfn.CONCAT(ROUND(L78, 2), " (", ROUND(N78,2), " - ", ROUND(M78,2),  ")", IF(AND(O78 &lt;0.05, NOT(ISBLANK(O78))), "*", " ") )</f>
         <v>1.01 (0.96 - 1.08)*</v>
       </c>
     </row>
@@ -18359,23 +18358,23 @@
         <v>5.7722744401177402E-63</v>
       </c>
       <c r="L80">
-        <f t="shared" ref="L80:L121" si="190">IFERROR(G80/G81,0)</f>
+        <f t="shared" ref="L80" si="190">IFERROR(G80/G81,0)</f>
         <v>1.3242009132415242</v>
       </c>
       <c r="M80">
-        <f t="shared" ref="M80:M120" si="191">IFERROR(H80/H81, 0)</f>
+        <f t="shared" ref="M80" si="191">IFERROR(H80/H81, 0)</f>
         <v>2.3747207090102829</v>
       </c>
       <c r="N80">
-        <f t="shared" ref="N80:N120" si="192">IFERROR(I80/I81, 0)</f>
+        <f t="shared" ref="N80" si="192">IFERROR(I80/I81, 0)</f>
         <v>0.98111617636475645</v>
       </c>
       <c r="O80">
-        <f t="shared" ref="O80:O120" si="193">IFERROR(J80/J81, 0)</f>
+        <f t="shared" ref="O80" si="193">IFERROR(J80/J81, 0)</f>
         <v>5.1118843147823643E-59</v>
       </c>
       <c r="Q80" t="str">
-        <f t="shared" ref="Q80:Q120" si="194">_xlfn.CONCAT(ROUND(L80, 2), " (", ROUND(N80,2), " - ", ROUND(M80,2),  ")", IF(AND(O80 &lt;0.05, NOT(ISBLANK(O80))), "*", " ") )</f>
+        <f t="shared" ref="Q80" si="194">_xlfn.CONCAT(ROUND(L80, 2), " (", ROUND(N80,2), " - ", ROUND(M80,2),  ")", IF(AND(O80 &lt;0.05, NOT(ISBLANK(O80))), "*", " ") )</f>
         <v>1.32 (0.98 - 2.37)*</v>
       </c>
     </row>
@@ -18463,23 +18462,23 @@
         <v>0</v>
       </c>
       <c r="L82">
-        <f t="shared" ref="L82:L121" si="195">IFERROR(G82/G83,0)</f>
+        <f t="shared" ref="L82" si="195">IFERROR(G82/G83,0)</f>
         <v>0.88336108324441998</v>
       </c>
       <c r="M82">
-        <f t="shared" ref="M82:M120" si="196">IFERROR(H82/H83, 0)</f>
+        <f t="shared" ref="M82" si="196">IFERROR(H82/H83, 0)</f>
         <v>0.90043517651829319</v>
       </c>
       <c r="N82">
-        <f t="shared" ref="N82:N120" si="197">IFERROR(I82/I83, 0)</f>
+        <f t="shared" ref="N82" si="197">IFERROR(I82/I83, 0)</f>
         <v>0.86757481377795453</v>
       </c>
       <c r="O82">
-        <f t="shared" ref="O82:O120" si="198">IFERROR(J82/J83, 0)</f>
+        <f t="shared" ref="O82" si="198">IFERROR(J82/J83, 0)</f>
         <v>0</v>
       </c>
       <c r="Q82" t="str">
-        <f t="shared" ref="Q82:Q120" si="199">_xlfn.CONCAT(ROUND(L82, 2), " (", ROUND(N82,2), " - ", ROUND(M82,2),  ")", IF(AND(O82 &lt;0.05, NOT(ISBLANK(O82))), "*", " ") )</f>
+        <f t="shared" ref="Q82" si="199">_xlfn.CONCAT(ROUND(L82, 2), " (", ROUND(N82,2), " - ", ROUND(M82,2),  ")", IF(AND(O82 &lt;0.05, NOT(ISBLANK(O82))), "*", " ") )</f>
         <v>0.88 (0.87 - 0.9)*</v>
       </c>
     </row>
@@ -18567,23 +18566,23 @@
         <v>0</v>
       </c>
       <c r="L84">
-        <f t="shared" ref="L84:L121" si="200">IFERROR(G84/G85,0)</f>
+        <f t="shared" ref="L84" si="200">IFERROR(G84/G85,0)</f>
         <v>0.95226979249042254</v>
       </c>
       <c r="M84">
-        <f t="shared" ref="M84:M120" si="201">IFERROR(H84/H85, 0)</f>
+        <f t="shared" ref="M84" si="201">IFERROR(H84/H85, 0)</f>
         <v>0.98158356811466829</v>
       </c>
       <c r="N84">
-        <f t="shared" ref="N84:N120" si="202">IFERROR(I84/I85, 0)</f>
+        <f t="shared" ref="N84" si="202">IFERROR(I84/I85, 0)</f>
         <v>0.9261243794246915</v>
       </c>
       <c r="O84">
-        <f t="shared" ref="O84:O120" si="203">IFERROR(J84/J85, 0)</f>
+        <f t="shared" ref="O84" si="203">IFERROR(J84/J85, 0)</f>
         <v>0</v>
       </c>
       <c r="Q84" t="str">
-        <f t="shared" ref="Q84:Q120" si="204">_xlfn.CONCAT(ROUND(L84, 2), " (", ROUND(N84,2), " - ", ROUND(M84,2),  ")", IF(AND(O84 &lt;0.05, NOT(ISBLANK(O84))), "*", " ") )</f>
+        <f t="shared" ref="Q84" si="204">_xlfn.CONCAT(ROUND(L84, 2), " (", ROUND(N84,2), " - ", ROUND(M84,2),  ")", IF(AND(O84 &lt;0.05, NOT(ISBLANK(O84))), "*", " ") )</f>
         <v>0.95 (0.93 - 0.98)*</v>
       </c>
     </row>
@@ -18671,23 +18670,23 @@
         <v>2.2859721815000399E-282</v>
       </c>
       <c r="L86">
-        <f t="shared" ref="L86:L121" si="205">IFERROR(G86/G87,0)</f>
+        <f t="shared" ref="L86" si="205">IFERROR(G86/G87,0)</f>
         <v>0.98635582822087542</v>
       </c>
       <c r="M86">
-        <f t="shared" ref="M86:M120" si="206">IFERROR(H86/H87, 0)</f>
+        <f t="shared" ref="M86" si="206">IFERROR(H86/H87, 0)</f>
         <v>1.0781796976857136</v>
       </c>
       <c r="N86">
-        <f t="shared" ref="N86:N120" si="207">IFERROR(I86/I87, 0)</f>
+        <f t="shared" ref="N86" si="207">IFERROR(I86/I87, 0)</f>
         <v>0.91638976183440757</v>
       </c>
       <c r="O86">
-        <f t="shared" ref="O86:O120" si="208">IFERROR(J86/J87, 0)</f>
+        <f t="shared" ref="O86" si="208">IFERROR(J86/J87, 0)</f>
         <v>2.1053244919759608E-235</v>
       </c>
       <c r="Q86" t="str">
-        <f t="shared" ref="Q86:Q120" si="209">_xlfn.CONCAT(ROUND(L86, 2), " (", ROUND(N86,2), " - ", ROUND(M86,2),  ")", IF(AND(O86 &lt;0.05, NOT(ISBLANK(O86))), "*", " ") )</f>
+        <f t="shared" ref="Q86" si="209">_xlfn.CONCAT(ROUND(L86, 2), " (", ROUND(N86,2), " - ", ROUND(M86,2),  ")", IF(AND(O86 &lt;0.05, NOT(ISBLANK(O86))), "*", " ") )</f>
         <v>0.99 (0.92 - 1.08)*</v>
       </c>
     </row>
@@ -18775,23 +18774,23 @@
         <v>0</v>
       </c>
       <c r="L88">
-        <f t="shared" ref="L88:L121" si="210">IFERROR(G88/G89,0)</f>
+        <f t="shared" ref="L88" si="210">IFERROR(G88/G89,0)</f>
         <v>0.95055270511126289</v>
       </c>
       <c r="M88">
-        <f t="shared" ref="M88:M120" si="211">IFERROR(H88/H89, 0)</f>
+        <f t="shared" ref="M88" si="211">IFERROR(H88/H89, 0)</f>
         <v>1.0128068536363386</v>
       </c>
       <c r="N88">
-        <f t="shared" ref="N88:N120" si="212">IFERROR(I88/I89, 0)</f>
+        <f t="shared" ref="N88" si="212">IFERROR(I88/I89, 0)</f>
         <v>0.90049718229083053</v>
       </c>
       <c r="O88">
-        <f t="shared" ref="O88:O120" si="213">IFERROR(J88/J89, 0)</f>
+        <f t="shared" ref="O88" si="213">IFERROR(J88/J89, 0)</f>
         <v>0</v>
       </c>
       <c r="Q88" t="str">
-        <f t="shared" ref="Q88:Q120" si="214">_xlfn.CONCAT(ROUND(L88, 2), " (", ROUND(N88,2), " - ", ROUND(M88,2),  ")", IF(AND(O88 &lt;0.05, NOT(ISBLANK(O88))), "*", " ") )</f>
+        <f t="shared" ref="Q88" si="214">_xlfn.CONCAT(ROUND(L88, 2), " (", ROUND(N88,2), " - ", ROUND(M88,2),  ")", IF(AND(O88 &lt;0.05, NOT(ISBLANK(O88))), "*", " ") )</f>
         <v>0.95 (0.9 - 1.01)*</v>
       </c>
     </row>
@@ -18879,23 +18878,23 @@
         <v>0</v>
       </c>
       <c r="L90">
-        <f t="shared" ref="L90:L121" si="215">IFERROR(G90/G91,0)</f>
+        <f t="shared" ref="L90" si="215">IFERROR(G90/G91,0)</f>
         <v>0.89541346939310495</v>
       </c>
       <c r="M90">
-        <f t="shared" ref="M90:M120" si="216">IFERROR(H90/H91, 0)</f>
+        <f t="shared" ref="M90" si="216">IFERROR(H90/H91, 0)</f>
         <v>0.92230695762096448</v>
       </c>
       <c r="N90">
-        <f t="shared" ref="N90:N120" si="217">IFERROR(I90/I91, 0)</f>
+        <f t="shared" ref="N90" si="217">IFERROR(I90/I91, 0)</f>
         <v>0.87149745534439615</v>
       </c>
       <c r="O90">
-        <f t="shared" ref="O90:O120" si="218">IFERROR(J90/J91, 0)</f>
+        <f t="shared" ref="O90" si="218">IFERROR(J90/J91, 0)</f>
         <v>0</v>
       </c>
       <c r="Q90" t="str">
-        <f t="shared" ref="Q90:Q120" si="219">_xlfn.CONCAT(ROUND(L90, 2), " (", ROUND(N90,2), " - ", ROUND(M90,2),  ")", IF(AND(O90 &lt;0.05, NOT(ISBLANK(O90))), "*", " ") )</f>
+        <f t="shared" ref="Q90" si="219">_xlfn.CONCAT(ROUND(L90, 2), " (", ROUND(N90,2), " - ", ROUND(M90,2),  ")", IF(AND(O90 &lt;0.05, NOT(ISBLANK(O90))), "*", " ") )</f>
         <v>0.9 (0.87 - 0.92)*</v>
       </c>
     </row>
@@ -18983,23 +18982,23 @@
         <v>0</v>
       </c>
       <c r="L92">
-        <f t="shared" ref="L92:L121" si="220">IFERROR(G92/G93,0)</f>
+        <f t="shared" ref="L92" si="220">IFERROR(G92/G93,0)</f>
         <v>1.0111537128096928</v>
       </c>
       <c r="M92">
-        <f t="shared" ref="M92:M120" si="221">IFERROR(H92/H93, 0)</f>
+        <f t="shared" ref="M92" si="221">IFERROR(H92/H93, 0)</f>
         <v>1.0584763611025949</v>
       </c>
       <c r="N92">
-        <f t="shared" ref="N92:N120" si="222">IFERROR(I92/I93, 0)</f>
+        <f t="shared" ref="N92" si="222">IFERROR(I92/I93, 0)</f>
         <v>0.97124187897000092</v>
       </c>
       <c r="O92">
-        <f t="shared" ref="O92:O120" si="223">IFERROR(J92/J93, 0)</f>
+        <f t="shared" ref="O92" si="223">IFERROR(J92/J93, 0)</f>
         <v>0</v>
       </c>
       <c r="Q92" t="str">
-        <f t="shared" ref="Q92:Q120" si="224">_xlfn.CONCAT(ROUND(L92, 2), " (", ROUND(N92,2), " - ", ROUND(M92,2),  ")", IF(AND(O92 &lt;0.05, NOT(ISBLANK(O92))), "*", " ") )</f>
+        <f t="shared" ref="Q92" si="224">_xlfn.CONCAT(ROUND(L92, 2), " (", ROUND(N92,2), " - ", ROUND(M92,2),  ")", IF(AND(O92 &lt;0.05, NOT(ISBLANK(O92))), "*", " ") )</f>
         <v>1.01 (0.97 - 1.06)*</v>
       </c>
     </row>
@@ -19087,23 +19086,23 @@
         <v>0</v>
       </c>
       <c r="L94">
-        <f t="shared" ref="L94:L121" si="225">IFERROR(G94/G95,0)</f>
+        <f t="shared" ref="L94" si="225">IFERROR(G94/G95,0)</f>
         <v>0.97692379923945527</v>
       </c>
       <c r="M94">
-        <f t="shared" ref="M94:M120" si="226">IFERROR(H94/H95, 0)</f>
+        <f t="shared" ref="M94" si="226">IFERROR(H94/H95, 0)</f>
         <v>1.0025524217527779</v>
       </c>
       <c r="N94">
-        <f t="shared" ref="N94:N120" si="227">IFERROR(I94/I95, 0)</f>
+        <f t="shared" ref="N94" si="227">IFERROR(I94/I95, 0)</f>
         <v>0.95398032084906148</v>
       </c>
       <c r="O94">
-        <f t="shared" ref="O94:O120" si="228">IFERROR(J94/J95, 0)</f>
+        <f t="shared" ref="O94" si="228">IFERROR(J94/J95, 0)</f>
         <v>0</v>
       </c>
       <c r="Q94" t="str">
-        <f t="shared" ref="Q94:Q120" si="229">_xlfn.CONCAT(ROUND(L94, 2), " (", ROUND(N94,2), " - ", ROUND(M94,2),  ")", IF(AND(O94 &lt;0.05, NOT(ISBLANK(O94))), "*", " ") )</f>
+        <f t="shared" ref="Q94" si="229">_xlfn.CONCAT(ROUND(L94, 2), " (", ROUND(N94,2), " - ", ROUND(M94,2),  ")", IF(AND(O94 &lt;0.05, NOT(ISBLANK(O94))), "*", " ") )</f>
         <v>0.98 (0.95 - 1)*</v>
       </c>
     </row>
@@ -19191,23 +19190,23 @@
         <v>0</v>
       </c>
       <c r="L96">
-        <f t="shared" ref="L96:L121" si="230">IFERROR(G96/G97,0)</f>
+        <f t="shared" ref="L96" si="230">IFERROR(G96/G97,0)</f>
         <v>0.96251778100099461</v>
       </c>
       <c r="M96">
-        <f t="shared" ref="M96:M120" si="231">IFERROR(H96/H97, 0)</f>
+        <f t="shared" ref="M96" si="231">IFERROR(H96/H97, 0)</f>
         <v>1.0102592567033009</v>
       </c>
       <c r="N96">
-        <f t="shared" ref="N96:N120" si="232">IFERROR(I96/I97, 0)</f>
+        <f t="shared" ref="N96" si="232">IFERROR(I96/I97, 0)</f>
         <v>0.92316577479430117</v>
       </c>
       <c r="O96">
-        <f t="shared" ref="O96:O120" si="233">IFERROR(J96/J97, 0)</f>
+        <f t="shared" ref="O96" si="233">IFERROR(J96/J97, 0)</f>
         <v>0</v>
       </c>
       <c r="Q96" t="str">
-        <f t="shared" ref="Q96:Q120" si="234">_xlfn.CONCAT(ROUND(L96, 2), " (", ROUND(N96,2), " - ", ROUND(M96,2),  ")", IF(AND(O96 &lt;0.05, NOT(ISBLANK(O96))), "*", " ") )</f>
+        <f t="shared" ref="Q96" si="234">_xlfn.CONCAT(ROUND(L96, 2), " (", ROUND(N96,2), " - ", ROUND(M96,2),  ")", IF(AND(O96 &lt;0.05, NOT(ISBLANK(O96))), "*", " ") )</f>
         <v>0.96 (0.92 - 1.01)*</v>
       </c>
     </row>
@@ -19295,23 +19294,23 @@
         <v>1.1685646151133201E-271</v>
       </c>
       <c r="L98">
-        <f t="shared" ref="L98:L121" si="235">IFERROR(G98/G99,0)</f>
+        <f t="shared" ref="L98" si="235">IFERROR(G98/G99,0)</f>
         <v>1.0325615763546705</v>
       </c>
       <c r="M98">
-        <f t="shared" ref="M98:M120" si="236">IFERROR(H98/H99, 0)</f>
+        <f t="shared" ref="M98" si="236">IFERROR(H98/H99, 0)</f>
         <v>1.0857872106688966</v>
       </c>
       <c r="N98">
-        <f t="shared" ref="N98:N120" si="237">IFERROR(I98/I99, 0)</f>
+        <f t="shared" ref="N98" si="237">IFERROR(I98/I99, 0)</f>
         <v>0.98918446633315726</v>
       </c>
       <c r="O98">
-        <f t="shared" ref="O98:O120" si="238">IFERROR(J98/J99, 0)</f>
+        <f t="shared" ref="O98" si="238">IFERROR(J98/J99, 0)</f>
         <v>5.1111583618310273E-190</v>
       </c>
       <c r="Q98" t="str">
-        <f t="shared" ref="Q98:Q120" si="239">_xlfn.CONCAT(ROUND(L98, 2), " (", ROUND(N98,2), " - ", ROUND(M98,2),  ")", IF(AND(O98 &lt;0.05, NOT(ISBLANK(O98))), "*", " ") )</f>
+        <f t="shared" ref="Q98" si="239">_xlfn.CONCAT(ROUND(L98, 2), " (", ROUND(N98,2), " - ", ROUND(M98,2),  ")", IF(AND(O98 &lt;0.05, NOT(ISBLANK(O98))), "*", " ") )</f>
         <v>1.03 (0.99 - 1.09)*</v>
       </c>
     </row>
@@ -19399,23 +19398,23 @@
         <v>2.19129240016169E-76</v>
       </c>
       <c r="L100">
-        <f t="shared" ref="L100:L121" si="240">IFERROR(G100/G101,0)</f>
+        <f t="shared" ref="L100" si="240">IFERROR(G100/G101,0)</f>
         <v>1.1177007299264181</v>
       </c>
       <c r="M100">
-        <f t="shared" ref="M100:M120" si="241">IFERROR(H100/H101, 0)</f>
+        <f t="shared" ref="M100" si="241">IFERROR(H100/H101, 0)</f>
         <v>1.4172107749115466</v>
       </c>
       <c r="N100">
-        <f t="shared" ref="N100:N120" si="242">IFERROR(I100/I101, 0)</f>
+        <f t="shared" ref="N100" si="242">IFERROR(I100/I101, 0)</f>
         <v>0.95461349521427574</v>
       </c>
       <c r="O100">
-        <f t="shared" ref="O100:O120" si="243">IFERROR(J100/J101, 0)</f>
+        <f t="shared" ref="O100" si="243">IFERROR(J100/J101, 0)</f>
         <v>7.278948099459065E-66</v>
       </c>
       <c r="Q100" t="str">
-        <f t="shared" ref="Q100:Q120" si="244">_xlfn.CONCAT(ROUND(L100, 2), " (", ROUND(N100,2), " - ", ROUND(M100,2),  ")", IF(AND(O100 &lt;0.05, NOT(ISBLANK(O100))), "*", " ") )</f>
+        <f t="shared" ref="Q100" si="244">_xlfn.CONCAT(ROUND(L100, 2), " (", ROUND(N100,2), " - ", ROUND(M100,2),  ")", IF(AND(O100 &lt;0.05, NOT(ISBLANK(O100))), "*", " ") )</f>
         <v>1.12 (0.95 - 1.42)*</v>
       </c>
     </row>
@@ -19503,23 +19502,23 @@
         <v>0</v>
       </c>
       <c r="L102">
-        <f t="shared" ref="L102:L121" si="245">IFERROR(G102/G103,0)</f>
+        <f t="shared" ref="L102" si="245">IFERROR(G102/G103,0)</f>
         <v>0.93216690975601835</v>
       </c>
       <c r="M102">
-        <f t="shared" ref="M102:M120" si="246">IFERROR(H102/H103, 0)</f>
+        <f t="shared" ref="M102" si="246">IFERROR(H102/H103, 0)</f>
         <v>0.94599255916892344</v>
       </c>
       <c r="N102">
-        <f t="shared" ref="N102:N120" si="247">IFERROR(I102/I103, 0)</f>
+        <f t="shared" ref="N102" si="247">IFERROR(I102/I103, 0)</f>
         <v>0.91925181168217507</v>
       </c>
       <c r="O102">
-        <f t="shared" ref="O102:O120" si="248">IFERROR(J102/J103, 0)</f>
+        <f t="shared" ref="O102" si="248">IFERROR(J102/J103, 0)</f>
         <v>0</v>
       </c>
       <c r="Q102" t="str">
-        <f t="shared" ref="Q102:Q120" si="249">_xlfn.CONCAT(ROUND(L102, 2), " (", ROUND(N102,2), " - ", ROUND(M102,2),  ")", IF(AND(O102 &lt;0.05, NOT(ISBLANK(O102))), "*", " ") )</f>
+        <f t="shared" ref="Q102" si="249">_xlfn.CONCAT(ROUND(L102, 2), " (", ROUND(N102,2), " - ", ROUND(M102,2),  ")", IF(AND(O102 &lt;0.05, NOT(ISBLANK(O102))), "*", " ") )</f>
         <v>0.93 (0.92 - 0.95)*</v>
       </c>
     </row>
@@ -19607,23 +19606,23 @@
         <v>0</v>
       </c>
       <c r="L104">
-        <f t="shared" ref="L104:L121" si="250">IFERROR(G104/G105,0)</f>
+        <f t="shared" ref="L104" si="250">IFERROR(G104/G105,0)</f>
         <v>1.1806348481308344</v>
       </c>
       <c r="M104">
-        <f t="shared" ref="M104:M120" si="251">IFERROR(H104/H105, 0)</f>
+        <f t="shared" ref="M104" si="251">IFERROR(H104/H105, 0)</f>
         <v>1.2607372613151104</v>
       </c>
       <c r="N104">
-        <f t="shared" ref="N104:N120" si="252">IFERROR(I104/I105, 0)</f>
+        <f t="shared" ref="N104" si="252">IFERROR(I104/I105, 0)</f>
         <v>1.1163649954262882</v>
       </c>
       <c r="O104">
-        <f t="shared" ref="O104:O120" si="253">IFERROR(J104/J105, 0)</f>
+        <f t="shared" ref="O104" si="253">IFERROR(J104/J105, 0)</f>
         <v>0</v>
       </c>
       <c r="Q104" t="str">
-        <f t="shared" ref="Q104:Q120" si="254">_xlfn.CONCAT(ROUND(L104, 2), " (", ROUND(N104,2), " - ", ROUND(M104,2),  ")", IF(AND(O104 &lt;0.05, NOT(ISBLANK(O104))), "*", " ") )</f>
+        <f t="shared" ref="Q104" si="254">_xlfn.CONCAT(ROUND(L104, 2), " (", ROUND(N104,2), " - ", ROUND(M104,2),  ")", IF(AND(O104 &lt;0.05, NOT(ISBLANK(O104))), "*", " ") )</f>
         <v>1.18 (1.12 - 1.26)*</v>
       </c>
     </row>
@@ -19711,23 +19710,23 @@
         <v>0</v>
       </c>
       <c r="L106">
-        <f t="shared" ref="L106:L121" si="255">IFERROR(G106/G107,0)</f>
+        <f t="shared" ref="L106" si="255">IFERROR(G106/G107,0)</f>
         <v>0.94978071918837192</v>
       </c>
       <c r="M106">
-        <f t="shared" ref="M106:M120" si="256">IFERROR(H106/H107, 0)</f>
+        <f t="shared" ref="M106" si="256">IFERROR(H106/H107, 0)</f>
         <v>0.97204813765557285</v>
       </c>
       <c r="N106">
-        <f t="shared" ref="N106:N120" si="257">IFERROR(I106/I107, 0)</f>
+        <f t="shared" ref="N106" si="257">IFERROR(I106/I107, 0)</f>
         <v>0.92957422737617668</v>
       </c>
       <c r="O106">
-        <f t="shared" ref="O106:O120" si="258">IFERROR(J106/J107, 0)</f>
+        <f t="shared" ref="O106" si="258">IFERROR(J106/J107, 0)</f>
         <v>0</v>
       </c>
       <c r="Q106" t="str">
-        <f t="shared" ref="Q106:Q120" si="259">_xlfn.CONCAT(ROUND(L106, 2), " (", ROUND(N106,2), " - ", ROUND(M106,2),  ")", IF(AND(O106 &lt;0.05, NOT(ISBLANK(O106))), "*", " ") )</f>
+        <f t="shared" ref="Q106" si="259">_xlfn.CONCAT(ROUND(L106, 2), " (", ROUND(N106,2), " - ", ROUND(M106,2),  ")", IF(AND(O106 &lt;0.05, NOT(ISBLANK(O106))), "*", " ") )</f>
         <v>0.95 (0.93 - 0.97)*</v>
       </c>
     </row>
@@ -19815,23 +19814,23 @@
         <v>6.7313073975867797E-240</v>
       </c>
       <c r="L108">
-        <f t="shared" ref="L108:L121" si="260">IFERROR(G108/G109,0)</f>
+        <f t="shared" ref="L108" si="260">IFERROR(G108/G109,0)</f>
         <v>1.1942616723432535</v>
       </c>
       <c r="M108">
-        <f t="shared" ref="M108:M120" si="261">IFERROR(H108/H109, 0)</f>
+        <f t="shared" ref="M108" si="261">IFERROR(H108/H109, 0)</f>
         <v>1.3011056561509595</v>
       </c>
       <c r="N108">
-        <f t="shared" ref="N108:N120" si="262">IFERROR(I108/I109, 0)</f>
+        <f t="shared" ref="N108" si="262">IFERROR(I108/I109, 0)</f>
         <v>1.1130843527818368</v>
       </c>
       <c r="O108">
-        <f t="shared" ref="O108:O120" si="263">IFERROR(J108/J109, 0)</f>
+        <f t="shared" ref="O108" si="263">IFERROR(J108/J109, 0)</f>
         <v>7.0632437846777763E-194</v>
       </c>
       <c r="Q108" t="str">
-        <f t="shared" ref="Q108:Q120" si="264">_xlfn.CONCAT(ROUND(L108, 2), " (", ROUND(N108,2), " - ", ROUND(M108,2),  ")", IF(AND(O108 &lt;0.05, NOT(ISBLANK(O108))), "*", " ") )</f>
+        <f t="shared" ref="Q108" si="264">_xlfn.CONCAT(ROUND(L108, 2), " (", ROUND(N108,2), " - ", ROUND(M108,2),  ")", IF(AND(O108 &lt;0.05, NOT(ISBLANK(O108))), "*", " ") )</f>
         <v>1.19 (1.11 - 1.3)*</v>
       </c>
     </row>
@@ -19919,23 +19918,23 @@
         <v>0</v>
       </c>
       <c r="L110">
-        <f t="shared" ref="L110:L121" si="265">IFERROR(G110/G111,0)</f>
+        <f t="shared" ref="L110" si="265">IFERROR(G110/G111,0)</f>
         <v>0.93270544584350623</v>
       </c>
       <c r="M110">
-        <f t="shared" ref="M110:M120" si="266">IFERROR(H110/H111, 0)</f>
+        <f t="shared" ref="M110" si="266">IFERROR(H110/H111, 0)</f>
         <v>0.94917382274114692</v>
       </c>
       <c r="N110">
-        <f t="shared" ref="N110:N120" si="267">IFERROR(I110/I111, 0)</f>
+        <f t="shared" ref="N110" si="267">IFERROR(I110/I111, 0)</f>
         <v>0.91771441798786002</v>
       </c>
       <c r="O110">
-        <f t="shared" ref="O110:O120" si="268">IFERROR(J110/J111, 0)</f>
+        <f t="shared" ref="O110" si="268">IFERROR(J110/J111, 0)</f>
         <v>0</v>
       </c>
       <c r="Q110" t="str">
-        <f t="shared" ref="Q110:Q120" si="269">_xlfn.CONCAT(ROUND(L110, 2), " (", ROUND(N110,2), " - ", ROUND(M110,2),  ")", IF(AND(O110 &lt;0.05, NOT(ISBLANK(O110))), "*", " ") )</f>
+        <f t="shared" ref="Q110" si="269">_xlfn.CONCAT(ROUND(L110, 2), " (", ROUND(N110,2), " - ", ROUND(M110,2),  ")", IF(AND(O110 &lt;0.05, NOT(ISBLANK(O110))), "*", " ") )</f>
         <v>0.93 (0.92 - 0.95)*</v>
       </c>
     </row>
@@ -20023,23 +20022,23 @@
         <v>6.2742425957564903E-103</v>
       </c>
       <c r="L112">
-        <f t="shared" ref="L112:L121" si="270">IFERROR(G112/G113,0)</f>
+        <f t="shared" ref="L112" si="270">IFERROR(G112/G113,0)</f>
         <v>1.2818787388171773</v>
       </c>
       <c r="M112">
-        <f t="shared" ref="M112:M120" si="271">IFERROR(H112/H113, 0)</f>
+        <f t="shared" ref="M112" si="271">IFERROR(H112/H113, 0)</f>
         <v>1.4370543543580165</v>
       </c>
       <c r="N112">
-        <f t="shared" ref="N112:N120" si="272">IFERROR(I112/I113, 0)</f>
+        <f t="shared" ref="N112" si="272">IFERROR(I112/I113, 0)</f>
         <v>1.1760663974561005</v>
       </c>
       <c r="O112">
-        <f t="shared" ref="O112:O120" si="273">IFERROR(J112/J113, 0)</f>
+        <f t="shared" ref="O112" si="273">IFERROR(J112/J113, 0)</f>
         <v>1.7085291087078754E-78</v>
       </c>
       <c r="Q112" t="str">
-        <f t="shared" ref="Q112:Q120" si="274">_xlfn.CONCAT(ROUND(L112, 2), " (", ROUND(N112,2), " - ", ROUND(M112,2),  ")", IF(AND(O112 &lt;0.05, NOT(ISBLANK(O112))), "*", " ") )</f>
+        <f t="shared" ref="Q112" si="274">_xlfn.CONCAT(ROUND(L112, 2), " (", ROUND(N112,2), " - ", ROUND(M112,2),  ")", IF(AND(O112 &lt;0.05, NOT(ISBLANK(O112))), "*", " ") )</f>
         <v>1.28 (1.18 - 1.44)*</v>
       </c>
     </row>
@@ -20127,23 +20126,23 @@
         <v>2.7294197558717899E-114</v>
       </c>
       <c r="L114">
-        <f t="shared" ref="L114:L121" si="275">IFERROR(G114/G115,0)</f>
+        <f t="shared" ref="L114" si="275">IFERROR(G114/G115,0)</f>
         <v>1.196635600436859</v>
       </c>
       <c r="M114">
-        <f t="shared" ref="M114:M120" si="276">IFERROR(H114/H115, 0)</f>
+        <f t="shared" ref="M114" si="276">IFERROR(H114/H115, 0)</f>
         <v>1.329914889234068</v>
       </c>
       <c r="N114">
-        <f t="shared" ref="N114:N120" si="277">IFERROR(I114/I115, 0)</f>
+        <f t="shared" ref="N114" si="277">IFERROR(I114/I115, 0)</f>
         <v>1.1036018117990072</v>
       </c>
       <c r="O114">
-        <f t="shared" ref="O114:O120" si="278">IFERROR(J114/J115, 0)</f>
+        <f t="shared" ref="O114" si="278">IFERROR(J114/J115, 0)</f>
         <v>9.0670657710544292E-87</v>
       </c>
       <c r="Q114" t="str">
-        <f t="shared" ref="Q114:Q120" si="279">_xlfn.CONCAT(ROUND(L114, 2), " (", ROUND(N114,2), " - ", ROUND(M114,2),  ")", IF(AND(O114 &lt;0.05, NOT(ISBLANK(O114))), "*", " ") )</f>
+        <f t="shared" ref="Q114" si="279">_xlfn.CONCAT(ROUND(L114, 2), " (", ROUND(N114,2), " - ", ROUND(M114,2),  ")", IF(AND(O114 &lt;0.05, NOT(ISBLANK(O114))), "*", " ") )</f>
         <v>1.2 (1.1 - 1.33)*</v>
       </c>
     </row>
@@ -20231,23 +20230,23 @@
         <v>6.2116372798042703E-12</v>
       </c>
       <c r="L116">
-        <f t="shared" ref="L116:L121" si="280">IFERROR(G116/G117,0)</f>
+        <f t="shared" ref="L116" si="280">IFERROR(G116/G117,0)</f>
         <v>1.3648170011823164</v>
       </c>
       <c r="M116">
-        <f t="shared" ref="M116:M120" si="281">IFERROR(H116/H117, 0)</f>
+        <f t="shared" ref="M116" si="281">IFERROR(H116/H117, 0)</f>
         <v>2.8725081636660255</v>
       </c>
       <c r="N116">
-        <f t="shared" ref="N116:N120" si="282">IFERROR(I116/I117, 0)</f>
+        <f t="shared" ref="N116" si="282">IFERROR(I116/I117, 0)</f>
         <v>1.0563715664330831</v>
       </c>
       <c r="O116">
-        <f t="shared" ref="O116:O120" si="283">IFERROR(J116/J117, 0)</f>
+        <f t="shared" ref="O116" si="283">IFERROR(J116/J117, 0)</f>
         <v>2.0734421893003796E-9</v>
       </c>
       <c r="Q116" t="str">
-        <f t="shared" ref="Q116:Q120" si="284">_xlfn.CONCAT(ROUND(L116, 2), " (", ROUND(N116,2), " - ", ROUND(M116,2),  ")", IF(AND(O116 &lt;0.05, NOT(ISBLANK(O116))), "*", " ") )</f>
+        <f t="shared" ref="Q116" si="284">_xlfn.CONCAT(ROUND(L116, 2), " (", ROUND(N116,2), " - ", ROUND(M116,2),  ")", IF(AND(O116 &lt;0.05, NOT(ISBLANK(O116))), "*", " ") )</f>
         <v>1.36 (1.06 - 2.87)*</v>
       </c>
     </row>
@@ -20335,23 +20334,23 @@
         <v>9.4888310316540696E-11</v>
       </c>
       <c r="L118">
-        <f t="shared" ref="L118:L121" si="285">IFERROR(G118/G119,0)</f>
+        <f t="shared" ref="L118" si="285">IFERROR(G118/G119,0)</f>
         <v>1.2857142857141197</v>
       </c>
       <c r="M118">
-        <f t="shared" ref="M118:M120" si="286">IFERROR(H118/H119, 0)</f>
+        <f t="shared" ref="M118" si="286">IFERROR(H118/H119, 0)</f>
         <v>0</v>
       </c>
       <c r="N118">
-        <f t="shared" ref="N118:N120" si="287">IFERROR(I118/I119, 0)</f>
+        <f t="shared" ref="N118" si="287">IFERROR(I118/I119, 0)</f>
         <v>1</v>
       </c>
       <c r="O118">
-        <f t="shared" ref="O118:O120" si="288">IFERROR(J118/J119, 0)</f>
+        <f t="shared" ref="O118" si="288">IFERROR(J118/J119, 0)</f>
         <v>5.1597294843696462E-10</v>
       </c>
       <c r="Q118" t="str">
-        <f t="shared" ref="Q118:Q120" si="289">_xlfn.CONCAT(ROUND(L118, 2), " (", ROUND(N118,2), " - ", ROUND(M118,2),  ")", IF(AND(O118 &lt;0.05, NOT(ISBLANK(O118))), "*", " ") )</f>
+        <f t="shared" ref="Q118" si="289">_xlfn.CONCAT(ROUND(L118, 2), " (", ROUND(N118,2), " - ", ROUND(M118,2),  ")", IF(AND(O118 &lt;0.05, NOT(ISBLANK(O118))), "*", " ") )</f>
         <v>1.29 (1 - 0)*</v>
       </c>
     </row>
@@ -20423,7 +20422,7 @@
         <v>100</v>
       </c>
       <c r="L120">
-        <f t="shared" ref="L120:L121" si="290">IFERROR(G120/G121,0)</f>
+        <f t="shared" ref="L120" si="290">IFERROR(G120/G121,0)</f>
         <v>0</v>
       </c>
       <c r="M120">
@@ -20485,7 +20484,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F568E0-A4E8-4E96-9684-88B9155E643F}">
   <dimension ref="B2:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="157" zoomScaleNormal="136" workbookViewId="0">
+    <sheetView zoomScale="157" zoomScaleNormal="136" workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
@@ -20499,17 +20498,17 @@
   <sheetData>
     <row r="2" spans="2:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="12" t="s">
+      <c r="C2" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D2" s="12"/>
-      <c r="E2" s="13" t="s">
+      <c r="D2" s="14"/>
+      <c r="E2" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+      <c r="I2" s="15"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -20545,7 +20544,7 @@
     </row>
     <row r="4" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="14" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -20578,7 +20577,7 @@
     </row>
     <row r="5" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
-      <c r="C5" s="13"/>
+      <c r="C5" s="15"/>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
@@ -20609,7 +20608,7 @@
     </row>
     <row r="6" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="14" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -20642,7 +20641,7 @@
     </row>
     <row r="7" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="C7" s="13"/>
+      <c r="C7" s="15"/>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
@@ -20673,7 +20672,7 @@
     </row>
     <row r="8" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="15" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -20706,7 +20705,7 @@
     </row>
     <row r="9" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="C9" s="13"/>
+      <c r="C9" s="15"/>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
@@ -20737,7 +20736,7 @@
     </row>
     <row r="10" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="14" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -20770,7 +20769,7 @@
     </row>
     <row r="11" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="C11" s="13"/>
+      <c r="C11" s="15"/>
       <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
@@ -20801,7 +20800,7 @@
     </row>
     <row r="12" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="15" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -20834,7 +20833,7 @@
     </row>
     <row r="13" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="13"/>
+      <c r="C13" s="15"/>
       <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
@@ -20865,7 +20864,7 @@
     </row>
     <row r="14" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="14" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -20898,7 +20897,7 @@
     </row>
     <row r="15" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="13"/>
+      <c r="C15" s="15"/>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>
@@ -21111,14 +21110,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="E2:I2"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C7"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="C8:C9"/>
     <mergeCell ref="C10:C11"/>
     <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:I2"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="C6:C7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Try controlling for hospital_id, results, no changes verified
</commit_message>
<xml_diff>
--- a/results/Paper/table_4.xlsx
+++ b/results/Paper/table_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C2BB2A3-D236-4A0B-8B5D-6BDB4FA48B94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31531E9B-BBB4-4C8F-98DF-26D273201B08}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
   </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
-    <pivotCache cacheId="1" r:id="rId6"/>
+    <pivotCache cacheId="0" r:id="rId6"/>
   </pivotCaches>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="527" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="52">
   <si>
     <t>cohort</t>
   </si>
@@ -195,12 +195,6 @@
     <t>race</t>
   </si>
   <si>
-    <t xml:space="preserve">Non-white </t>
-  </si>
-  <si>
-    <t xml:space="preserve">White </t>
-  </si>
-  <si>
     <t>No Ventilation</t>
   </si>
   <si>
@@ -216,9 +210,6 @@
     <t>Grand Total</t>
   </si>
   <si>
-    <t>Average of psi</t>
-  </si>
-  <si>
     <t>ratio_psi</t>
   </si>
   <si>
@@ -231,11 +222,20 @@
     <t>ATE Ratio
 White vs. Non-White</t>
   </si>
+  <si>
+    <t>(All)</t>
+  </si>
+  <si>
+    <t>Average of ATE</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="169" formatCode="0.000"/>
+  </numFmts>
   <fonts count="20" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -787,8 +787,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" indent="2"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -796,12 +799,7 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
+    <xf numFmtId="169" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -847,7 +845,64 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="14">
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="169" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -2251,8 +2306,8 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable29" cacheId="1" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
-  <location ref="N4:O47" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable29" cacheId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="8" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="8" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="N4:O23" firstHeaderRow="1" firstDataRow="1" firstDataCol="1" rowPageCount="2" colPageCount="1"/>
   <pivotFields count="9">
     <pivotField axis="axisRow" showAll="0">
       <items count="7">
@@ -2267,15 +2322,15 @@
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
-        <item x="0"/>
-        <item x="1"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
     <pivotField axis="axisRow" showAll="0">
       <items count="3">
-        <item x="0"/>
-        <item x="1"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="1"/>
         <item t="default"/>
       </items>
     </pivotField>
@@ -2307,26 +2362,14 @@
     <field x="2"/>
     <field x="1"/>
   </rowFields>
-  <rowItems count="43">
+  <rowItems count="19">
     <i>
       <x/>
     </i>
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i>
@@ -2335,19 +2378,7 @@
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i>
@@ -2356,19 +2387,7 @@
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i>
@@ -2377,19 +2396,7 @@
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i>
@@ -2398,19 +2405,7 @@
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i>
@@ -2419,19 +2414,7 @@
     <i r="1">
       <x/>
     </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
-      <x v="1"/>
-    </i>
     <i r="1">
-      <x v="1"/>
-    </i>
-    <i r="2">
-      <x/>
-    </i>
-    <i r="2">
       <x v="1"/>
     </i>
     <i t="grand">
@@ -2442,12 +2425,20 @@
     <i/>
   </colItems>
   <pageFields count="2">
-    <pageField fld="3" item="1" hier="-1"/>
-    <pageField fld="4" item="1" hier="-1"/>
+    <pageField fld="3" hier="-1"/>
+    <pageField fld="4" hier="-1"/>
   </pageFields>
   <dataFields count="1">
-    <dataField name="Average of psi" fld="5" subtotal="average" baseField="2" baseItem="0"/>
+    <dataField name="Average of ATE" fld="5" subtotal="average" baseField="2" baseItem="0" numFmtId="169"/>
   </dataFields>
+  <formats count="2">
+    <format dxfId="13">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+    <format dxfId="12">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
   <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
@@ -7377,8 +7368,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:O121"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="Q22" sqref="Q22"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="115" workbookViewId="0">
+      <selection activeCell="Q25" sqref="Q25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7389,8 +7380,8 @@
     <col min="5" max="9" width="9" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="13.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="15.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17.5546875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="13.21875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="16.77734375" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="13.88671875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="15.33203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="15.88671875" bestFit="1" customWidth="1"/>
   </cols>
@@ -7427,8 +7418,8 @@
       <c r="N1" s="8" t="s">
         <v>3</v>
       </c>
-      <c r="O1" s="9">
-        <v>6</v>
+      <c r="O1" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.3">
@@ -7479,8 +7470,8 @@
       <c r="N2" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="O2" s="9">
-        <v>10</v>
+      <c r="O2" t="s">
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
@@ -7575,10 +7566,10 @@
         <v>0.51 (0.48 - 0.54)*</v>
       </c>
       <c r="N4" s="8" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="O4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
@@ -7629,8 +7620,8 @@
       <c r="N5" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="O5">
-        <v>0.38408227893435404</v>
+      <c r="O5" s="15">
+        <v>0.45735875431667772</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
@@ -7681,8 +7672,8 @@
       <c r="N6" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="O6">
-        <v>0.48164705582437051</v>
+      <c r="O6" s="15">
+        <v>0.52703305678788903</v>
       </c>
     </row>
     <row r="7" spans="1:15" x14ac:dyDescent="0.3">
@@ -7730,11 +7721,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G7, 2), " (", ROUND(temp!H7,2), " - ", ROUND(temp!I7,2),  ")", IF(AND(temp!J7 &lt;0.05, NOT(ISBLANK(temp!J7))), "*", " ") )</f>
         <v>0.27 (0.25 - 0.29)*</v>
       </c>
-      <c r="N7" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7">
-        <v>0.51160443995962901</v>
+      <c r="N7" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O7" s="15">
+        <v>0.38768445184546652</v>
       </c>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
@@ -7782,11 +7773,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G8, 2), " (", ROUND(temp!H8,2), " - ", ROUND(temp!I8,2),  ")", IF(AND(temp!J8 &lt;0.05, NOT(ISBLANK(temp!J8))), "*", " ") )</f>
         <v>0.19 (0.16 - 0.21)*</v>
       </c>
-      <c r="N8" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O8">
-        <v>0.451689671689112</v>
+      <c r="N8" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="O8" s="15">
+        <v>0.48861975555631554</v>
       </c>
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.3">
@@ -7835,10 +7826,10 @@
         <v>0.29 (0.26 - 0.31)*</v>
       </c>
       <c r="N9" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O9">
-        <v>0.28651750204433751</v>
+        <v>20</v>
+      </c>
+      <c r="O9" s="15">
+        <v>0.63211375225250666</v>
       </c>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
@@ -7886,11 +7877,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G10, 2), " (", ROUND(temp!H10,2), " - ", ROUND(temp!I10,2),  ")", IF(AND(temp!J10 &lt;0.05, NOT(ISBLANK(temp!J10))), "*", " ") )</f>
         <v>0.53 (0.48 - 0.59)*</v>
       </c>
-      <c r="N10" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10">
-        <v>0.28655959425226002</v>
+      <c r="N10" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O10" s="15">
+        <v>0.34512575886012442</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.3">
@@ -7938,11 +7929,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G11, 2), " (", ROUND(temp!H11,2), " - ", ROUND(temp!I11,2),  ")", IF(AND(temp!J11 &lt;0.05, NOT(ISBLANK(temp!J11))), "*", " ") )</f>
         <v>0.64 (0.45 - 0.83)*</v>
       </c>
-      <c r="N11" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O11">
-        <v>0.28647540983641501</v>
+      <c r="N11" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="O11" s="15">
+        <v>0.50744104716905869</v>
       </c>
     </row>
     <row r="12" spans="1:15" x14ac:dyDescent="0.3">
@@ -7990,11 +7981,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G12, 2), " (", ROUND(temp!H12,2), " - ", ROUND(temp!I12,2),  ")", IF(AND(temp!J12 &lt;0.05, NOT(ISBLANK(temp!J12))), "*", " ") )</f>
         <v>0.45 (0.44 - 0.46)*</v>
       </c>
-      <c r="N12" s="9" t="s">
-        <v>43</v>
-      </c>
-      <c r="O12">
-        <v>0.37191644982658001</v>
+      <c r="N12" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O12" s="15">
+        <v>0.67427941842462968</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
@@ -8043,10 +8034,10 @@
         <v>0.29 (0.27 - 0.31)*</v>
       </c>
       <c r="N13" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O13">
-        <v>0.59614733495410555</v>
+        <v>11</v>
+      </c>
+      <c r="O13" s="15">
+        <v>0.34060267591348747</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
@@ -8094,11 +8085,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G14, 2), " (", ROUND(temp!H14,2), " - ", ROUND(temp!I14,2),  ")", IF(AND(temp!J14 &lt;0.05, NOT(ISBLANK(temp!J14))), "*", " ") )</f>
         <v>0.45 (0.44 - 0.47)*</v>
       </c>
-      <c r="N14" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O14">
-        <v>0.61925795053003196</v>
+      <c r="N14" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="O14" s="15">
+        <v>0.45324760017548016</v>
       </c>
     </row>
     <row r="15" spans="1:15" x14ac:dyDescent="0.3">
@@ -8146,11 +8137,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G15, 2), " (", ROUND(temp!H15,2), " - ", ROUND(temp!I15,2),  ")", IF(AND(temp!J15 &lt;0.05, NOT(ISBLANK(temp!J15))), "*", " ") )</f>
         <v>0.63 (0.61 - 0.65)*</v>
       </c>
-      <c r="N15" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O15">
-        <v>0.57303671937817902</v>
+      <c r="N15" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O15" s="15">
+        <v>0.56245659823410554</v>
       </c>
     </row>
     <row r="16" spans="1:15" x14ac:dyDescent="0.3">
@@ -8201,8 +8192,8 @@
       <c r="N16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="O16">
-        <v>0.1476855646990545</v>
+      <c r="O16" s="15">
+        <v>0.34403860211685494</v>
       </c>
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.3">
@@ -8250,11 +8241,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G17, 2), " (", ROUND(temp!H17,2), " - ", ROUND(temp!I17,2),  ")", IF(AND(temp!J17 &lt;0.05, NOT(ISBLANK(temp!J17))), "*", " ") )</f>
         <v>0.27 (0.26 - 0.27)*</v>
       </c>
-      <c r="N17" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O17">
-        <v>0.1321499013812</v>
+      <c r="N17" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="O17" s="15">
+        <v>0.46469298913159279</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.3">
@@ -8302,11 +8293,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G18, 2), " (", ROUND(temp!H18,2), " - ", ROUND(temp!I18,2),  ")", IF(AND(temp!J18 &lt;0.05, NOT(ISBLANK(temp!J18))), "*", " ") )</f>
         <v>0.19 (0.18 - 0.2)*</v>
       </c>
-      <c r="N18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O18">
-        <v>0.163221228016909</v>
+      <c r="N18" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O18" s="15">
+        <v>0.53498412385747296</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.3">
@@ -8354,11 +8345,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G19, 2), " (", ROUND(temp!H19,2), " - ", ROUND(temp!I19,2),  ")", IF(AND(temp!J19 &lt;0.05, NOT(ISBLANK(temp!J19))), "*", " ") )</f>
         <v>0.29 (0.27 - 0.3)*</v>
       </c>
-      <c r="N19" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="O19">
-        <v>0.46311959728281249</v>
+      <c r="N19" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O19" s="15">
+        <v>0.39440185440571246</v>
       </c>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.3">
@@ -8406,11 +8397,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G20, 2), " (", ROUND(temp!H20,2), " - ", ROUND(temp!I20,2),  ")", IF(AND(temp!J20 &lt;0.05, NOT(ISBLANK(temp!J20))), "*", " ") )</f>
         <v>0.5 (0.48 - 0.53)*</v>
       </c>
-      <c r="N20" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O20">
-        <v>0.69002365571811208</v>
+      <c r="N20" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="O20" s="15">
+        <v>0.40878609454430637</v>
       </c>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.3">
@@ -8458,11 +8449,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G21, 2), " (", ROUND(temp!H21,2), " - ", ROUND(temp!I21,2),  ")", IF(AND(temp!J21 &lt;0.05, NOT(ISBLANK(temp!J21))), "*", " ") )</f>
         <v>0.71 (0.63 - 0.79)*</v>
       </c>
-      <c r="N21" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O21">
-        <v>0.66896551724132902</v>
+      <c r="N21" s="10" t="s">
+        <v>20</v>
+      </c>
+      <c r="O21" s="15">
+        <v>0.58090065261797685</v>
       </c>
     </row>
     <row r="22" spans="1:15" x14ac:dyDescent="0.3">
@@ -8510,11 +8501,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G22, 2), " (", ROUND(temp!H22,2), " - ", ROUND(temp!I22,2),  ")", IF(AND(temp!J22 &lt;0.05, NOT(ISBLANK(temp!J22))), "*", " ") )</f>
         <v>0.52 (0.5 - 0.54)*</v>
       </c>
-      <c r="N22" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O22">
-        <v>0.71108179419489503</v>
+      <c r="N22" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="O22" s="15">
+        <v>0.23667153647063582</v>
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.3">
@@ -8562,11 +8553,11 @@
         <f>_xlfn.CONCAT(ROUND(temp!G23, 2), " (", ROUND(temp!H23,2), " - ", ROUND(temp!I23,2),  ")", IF(AND(temp!J23 &lt;0.05, NOT(ISBLANK(temp!J23))), "*", " ") )</f>
         <v>0.44 (0.42 - 0.47)*</v>
       </c>
-      <c r="N23" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O23">
-        <v>0.23621553884751301</v>
+      <c r="N23" s="9" t="s">
+        <v>45</v>
+      </c>
+      <c r="O23" s="15">
+        <v>0.46335770681557215</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.3">
@@ -8614,12 +8605,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G24, 2), " (", ROUND(temp!H24,2), " - ", ROUND(temp!I24,2),  ")", IF(AND(temp!J24 &lt;0.05, NOT(ISBLANK(temp!J24))), "*", " ") )</f>
         <v>0.62 (0.59 - 0.65)*</v>
       </c>
-      <c r="N24" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O24">
-        <v>0.21491228070193999</v>
-      </c>
     </row>
     <row r="25" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A25">
@@ -8666,12 +8651,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G25, 2), " (", ROUND(temp!H25,2), " - ", ROUND(temp!I25,2),  ")", IF(AND(temp!J25 &lt;0.05, NOT(ISBLANK(temp!J25))), "*", " ") )</f>
         <v>0.8 (0.73 - 0.87)*</v>
       </c>
-      <c r="N25" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O25">
-        <v>0.257518796993086</v>
-      </c>
     </row>
     <row r="26" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A26">
@@ -8718,12 +8697,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G26, 2), " (", ROUND(temp!H26,2), " - ", ROUND(temp!I26,2),  ")", IF(AND(temp!J26 &lt;0.05, NOT(ISBLANK(temp!J26))), "*", " ") )</f>
         <v>0.8 (0.55 - 1)*</v>
       </c>
-      <c r="N26" s="9" t="s">
-        <v>44</v>
-      </c>
-      <c r="O26">
-        <v>0.37006554197770503</v>
-      </c>
     </row>
     <row r="27" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A27">
@@ -8770,12 +8743,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G27, 2), " (", ROUND(temp!H27,2), " - ", ROUND(temp!I27,2),  ")", IF(AND(temp!J27 &lt;0.05, NOT(ISBLANK(temp!J27))), "*", " ") )</f>
         <v>0.08 (0.07 - 0.09)*</v>
       </c>
-      <c r="N27" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O27">
-        <v>0.51531660251544653</v>
-      </c>
     </row>
     <row r="28" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A28">
@@ -8822,12 +8789,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G28, 2), " (", ROUND(temp!H28,2), " - ", ROUND(temp!I28,2),  ")", IF(AND(temp!J28 &lt;0.05, NOT(ISBLANK(temp!J28))), "*", " ") )</f>
         <v>0.06 (0.05 - 0.07)*</v>
       </c>
-      <c r="N28" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O28">
-        <v>0.54324644544899903</v>
-      </c>
     </row>
     <row r="29" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A29">
@@ -8874,12 +8835,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G29, 2), " (", ROUND(temp!H29,2), " - ", ROUND(temp!I29,2),  ")", IF(AND(temp!J29 &lt;0.05, NOT(ISBLANK(temp!J29))), "*", " ") )</f>
         <v>0.13 (0.11 - 0.15)*</v>
       </c>
-      <c r="N29" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O29">
-        <v>0.48738675958189398</v>
-      </c>
     </row>
     <row r="30" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A30">
@@ -8926,12 +8881,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G30, 2), " (", ROUND(temp!H30,2), " - ", ROUND(temp!I30,2),  ")", IF(AND(temp!J30 &lt;0.05, NOT(ISBLANK(temp!J30))), "*", " ") )</f>
         <v>0.37 (0.23 - 0.5)*</v>
       </c>
-      <c r="N30" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O30">
-        <v>0.22481448143996349</v>
-      </c>
     </row>
     <row r="31" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A31">
@@ -8978,12 +8927,6 @@
         <f>_xlfn.CONCAT(ROUND(temp!G31, 2), " (", ROUND(temp!H31,2), " - ", ROUND(temp!I31,2),  ")", IF(AND(temp!J31 &lt;0.05, NOT(ISBLANK(temp!J31))), "*", " ") )</f>
         <v xml:space="preserve">1 (0 - 1) </v>
       </c>
-      <c r="N31" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O31">
-        <v>0.215393452039258</v>
-      </c>
     </row>
     <row r="32" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A32">
@@ -9030,14 +8973,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G32, 2), " (", ROUND(temp!H32,2), " - ", ROUND(temp!I32,2),  ")", IF(AND(temp!J32 &lt;0.05, NOT(ISBLANK(temp!J32))), "*", " ") )</f>
         <v>0.48 (0.48 - 0.49)*</v>
       </c>
-      <c r="N32" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O32">
-        <v>0.23423551084066899</v>
-      </c>
-    </row>
-    <row r="33" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A33">
         <f>LTMLE!A73</f>
         <v>72</v>
@@ -9082,14 +9019,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G33, 2), " (", ROUND(temp!H33,2), " - ", ROUND(temp!I33,2),  ")", IF(AND(temp!J33 &lt;0.05, NOT(ISBLANK(temp!J33))), "*", " ") )</f>
         <v>0.42 (0.41 - 0.43)*</v>
       </c>
-      <c r="N33" s="9" t="s">
-        <v>25</v>
-      </c>
-      <c r="O33">
-        <v>0.3935388940891873</v>
-      </c>
-    </row>
-    <row r="34" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A34">
         <f>LTMLE!A74</f>
         <v>73</v>
@@ -9134,14 +9065,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G34, 2), " (", ROUND(temp!H34,2), " - ", ROUND(temp!I34,2),  ")", IF(AND(temp!J34 &lt;0.05, NOT(ISBLANK(temp!J34))), "*", " ") )</f>
         <v>0.57 (0.56 - 0.59)*</v>
       </c>
-      <c r="N34" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O34">
-        <v>0.49365482001656452</v>
-      </c>
-    </row>
-    <row r="35" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A35">
         <f>LTMLE!A75</f>
         <v>74</v>
@@ -9186,14 +9111,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G35, 2), " (", ROUND(temp!H35,2), " - ", ROUND(temp!I35,2),  ")", IF(AND(temp!J35 &lt;0.05, NOT(ISBLANK(temp!J35))), "*", " ") )</f>
         <v>0.77 (0.73 - 0.81)*</v>
       </c>
-      <c r="N35" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O35">
-        <v>0.52089407191416504</v>
-      </c>
-    </row>
-    <row r="36" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A36">
         <f>LTMLE!A76</f>
         <v>75</v>
@@ -9238,14 +9157,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G36, 2), " (", ROUND(temp!H36,2), " - ", ROUND(temp!I36,2),  ")", IF(AND(temp!J36 &lt;0.05, NOT(ISBLANK(temp!J36))), "*", " ") )</f>
         <v>0.88 (0.75 - 1)*</v>
       </c>
-      <c r="N36" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O36">
-        <v>0.46641556811896401</v>
-      </c>
-    </row>
-    <row r="37" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A37">
         <f>LTMLE!A12</f>
         <v>11</v>
@@ -9290,14 +9203,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G37, 2), " (", ROUND(temp!H37,2), " - ", ROUND(temp!I37,2),  ")", IF(AND(temp!J37 &lt;0.05, NOT(ISBLANK(temp!J37))), "*", " ") )</f>
         <v>0.09 (0.09 - 0.1)*</v>
       </c>
-      <c r="N37" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O37">
-        <v>0.29342296816181002</v>
-      </c>
-    </row>
-    <row r="38" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A38">
         <f>LTMLE!A13</f>
         <v>12</v>
@@ -9342,14 +9249,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G38, 2), " (", ROUND(temp!H38,2), " - ", ROUND(temp!I38,2),  ")", IF(AND(temp!J38 &lt;0.05, NOT(ISBLANK(temp!J38))), "*", " ") )</f>
         <v>0.07 (0.07 - 0.08)*</v>
       </c>
-      <c r="N38" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O38">
-        <v>0.29179566563500697</v>
-      </c>
-    </row>
-    <row r="39" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="39" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A39">
         <f>LTMLE!A14</f>
         <v>13</v>
@@ -9394,14 +9295,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G39, 2), " (", ROUND(temp!H39,2), " - ", ROUND(temp!I39,2),  ")", IF(AND(temp!J39 &lt;0.05, NOT(ISBLANK(temp!J39))), "*", " ") )</f>
         <v>0.16 (0.15 - 0.18)*</v>
       </c>
-      <c r="N39" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O39">
-        <v>0.295050270688613</v>
-      </c>
-    </row>
-    <row r="40" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="40" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A40">
         <f>LTMLE!A15</f>
         <v>14</v>
@@ -9446,14 +9341,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G40, 2), " (", ROUND(temp!H40,2), " - ", ROUND(temp!I40,2),  ")", IF(AND(temp!J40 &lt;0.05, NOT(ISBLANK(temp!J40))), "*", " ") )</f>
         <v>0.48 (0.41 - 0.55)*</v>
       </c>
-      <c r="N40" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="O40">
-        <v>0.35730962902056324</v>
-      </c>
-    </row>
-    <row r="41" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A41">
         <f>LTMLE!A16</f>
         <v>15</v>
@@ -9498,14 +9387,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G41, 2), " (", ROUND(temp!H41,2), " - ", ROUND(temp!I41,2),  ")", IF(AND(temp!J41 &lt;0.05, NOT(ISBLANK(temp!J41))), "*", " ") )</f>
         <v>1 (1 - 1)*</v>
       </c>
-      <c r="N41" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="O41">
-        <v>0.59359143492087996</v>
-      </c>
-    </row>
-    <row r="42" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A42">
         <f>LTMLE!A87</f>
         <v>86</v>
@@ -9550,14 +9433,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G42, 2), " (", ROUND(temp!H42,2), " - ", ROUND(temp!I42,2),  ")", IF(AND(temp!J42 &lt;0.05, NOT(ISBLANK(temp!J42))), "*", " ") )</f>
         <v>0.67 (0.64 - 0.7)*</v>
       </c>
-      <c r="N42" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O42">
-        <v>0.61425959780623896</v>
-      </c>
-    </row>
-    <row r="43" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A43">
         <f>LTMLE!A88</f>
         <v>87</v>
@@ -9602,14 +9479,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G43, 2), " (", ROUND(temp!H43,2), " - ", ROUND(temp!I43,2),  ")", IF(AND(temp!J43 &lt;0.05, NOT(ISBLANK(temp!J43))), "*", " ") )</f>
         <v>0.6 (0.52 - 0.68)*</v>
       </c>
-      <c r="N43" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O43">
-        <v>0.57292327203552096</v>
-      </c>
-    </row>
-    <row r="44" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="44" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A44">
         <f>LTMLE!A89</f>
         <v>88</v>
@@ -9654,14 +9525,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G44, 2), " (", ROUND(temp!H44,2), " - ", ROUND(temp!I44,2),  ")", IF(AND(temp!J44 &lt;0.05, NOT(ISBLANK(temp!J44))), "*", " ") )</f>
         <v>0.67 (0.62 - 0.71)*</v>
       </c>
-      <c r="N44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="O44">
-        <v>0.12102782312024651</v>
-      </c>
-    </row>
-    <row r="45" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="45" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A45">
         <f>LTMLE!A90</f>
         <v>89</v>
@@ -9706,14 +9571,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G45, 2), " (", ROUND(temp!H45,2), " - ", ROUND(temp!I45,2),  ")", IF(AND(temp!J45 &lt;0.05, NOT(ISBLANK(temp!J45))), "*", " ") )</f>
         <v>0.71 (0.65 - 0.77)*</v>
       </c>
-      <c r="N45" s="11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O45">
-        <v>0.106077348512377</v>
-      </c>
-    </row>
-    <row r="46" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="46" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A46">
         <f>LTMLE!A91</f>
         <v>90</v>
@@ -9758,14 +9617,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G46, 2), " (", ROUND(temp!H46,2), " - ", ROUND(temp!I46,2),  ")", IF(AND(temp!J46 &lt;0.05, NOT(ISBLANK(temp!J46))), "*", " ") )</f>
         <v>0.68 (0.57 - 0.78)*</v>
       </c>
-      <c r="N46" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="O46">
-        <v>0.13597829772811601</v>
-      </c>
-    </row>
-    <row r="47" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="47" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A47">
         <f>LTMLE!A27</f>
         <v>26</v>
@@ -9810,14 +9663,8 @@
         <f>_xlfn.CONCAT(ROUND(temp!G47, 2), " (", ROUND(temp!H47,2), " - ", ROUND(temp!I47,2),  ")", IF(AND(temp!J47 &lt;0.05, NOT(ISBLANK(temp!J47))), "*", " ") )</f>
         <v>0.22 (0.19 - 0.25)*</v>
       </c>
-      <c r="N47" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="O47">
-        <v>0.390005398521867</v>
-      </c>
-    </row>
-    <row r="48" spans="1:15" x14ac:dyDescent="0.3">
+    </row>
+    <row r="48" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A48">
         <f>LTMLE!A28</f>
         <v>27</v>
@@ -13197,6 +13044,7 @@
     <sortCondition ref="E2:E122"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
@@ -13218,18 +13066,18 @@
   <sheetData>
     <row r="3" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="15" t="s">
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="G3" s="15"/>
-      <c r="H3" s="15"/>
-      <c r="I3" s="15"/>
-      <c r="J3" s="15"/>
+      <c r="G3" s="11"/>
+      <c r="H3" s="11"/>
+      <c r="I3" s="11"/>
+      <c r="J3" s="11"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
       <c r="M3" s="2"/>
@@ -13268,10 +13116,10 @@
     </row>
     <row r="5" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E5" s="4" t="s">
@@ -13300,8 +13148,8 @@
     </row>
     <row r="6" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="14"/>
       <c r="E6" s="4" t="s">
         <v>11</v>
       </c>
@@ -13328,8 +13176,8 @@
     </row>
     <row r="7" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12" t="s">
+      <c r="C7" s="11"/>
+      <c r="D7" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E7" s="4" t="s">
@@ -13358,8 +13206,8 @@
     </row>
     <row r="8" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="C8" s="15"/>
-      <c r="D8" s="13"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="14"/>
       <c r="E8" s="4" t="s">
         <v>11</v>
       </c>
@@ -13386,10 +13234,10 @@
     </row>
     <row r="9" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E9" s="4" t="s">
@@ -13418,8 +13266,8 @@
     </row>
     <row r="10" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="C10" s="15"/>
-      <c r="D10" s="13"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="14"/>
       <c r="E10" s="4" t="s">
         <v>11</v>
       </c>
@@ -13446,8 +13294,8 @@
     </row>
     <row r="11" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12" t="s">
+      <c r="C11" s="11"/>
+      <c r="D11" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E11" s="4" t="s">
@@ -13476,8 +13324,8 @@
     </row>
     <row r="12" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="13"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="14"/>
       <c r="E12" s="4" t="s">
         <v>11</v>
       </c>
@@ -13504,10 +13352,10 @@
     </row>
     <row r="13" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E13" s="4" t="s">
@@ -13536,8 +13384,8 @@
     </row>
     <row r="14" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="13"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="14"/>
       <c r="E14" s="4" t="s">
         <v>11</v>
       </c>
@@ -13564,8 +13412,8 @@
     </row>
     <row r="15" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="12" t="s">
+      <c r="C15" s="11"/>
+      <c r="D15" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E15" s="4" t="s">
@@ -13594,8 +13442,8 @@
     </row>
     <row r="16" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="13"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="14"/>
       <c r="E16" s="4" t="s">
         <v>11</v>
       </c>
@@ -13622,10 +13470,10 @@
     </row>
     <row r="17" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B17" s="2"/>
-      <c r="C17" s="14" t="s">
+      <c r="C17" s="12" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="4" t="s">
@@ -13654,8 +13502,8 @@
     </row>
     <row r="18" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B18" s="2"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="14"/>
       <c r="E18" s="4" t="s">
         <v>11</v>
       </c>
@@ -13682,8 +13530,8 @@
     </row>
     <row r="19" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B19" s="2"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="12" t="s">
+      <c r="C19" s="11"/>
+      <c r="D19" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E19" s="4" t="s">
@@ -13712,8 +13560,8 @@
     </row>
     <row r="20" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B20" s="2"/>
-      <c r="C20" s="15"/>
-      <c r="D20" s="13"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="14"/>
       <c r="E20" s="4" t="s">
         <v>11</v>
       </c>
@@ -13740,10 +13588,10 @@
     </row>
     <row r="21" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B21" s="2"/>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E21" s="4" t="s">
@@ -13772,8 +13620,8 @@
     </row>
     <row r="22" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B22" s="2"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="13"/>
+      <c r="C22" s="11"/>
+      <c r="D22" s="14"/>
       <c r="E22" s="4" t="s">
         <v>11</v>
       </c>
@@ -13800,8 +13648,8 @@
     </row>
     <row r="23" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B23" s="2"/>
-      <c r="C23" s="15"/>
-      <c r="D23" s="12" t="s">
+      <c r="C23" s="11"/>
+      <c r="D23" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E23" s="4" t="s">
@@ -13830,8 +13678,8 @@
     </row>
     <row r="24" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B24" s="2"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="13"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="14"/>
       <c r="E24" s="4" t="s">
         <v>11</v>
       </c>
@@ -13858,10 +13706,10 @@
     </row>
     <row r="25" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B25" s="2"/>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="13" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="4" t="s">
@@ -13890,8 +13738,8 @@
     </row>
     <row r="26" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B26" s="2"/>
-      <c r="C26" s="15"/>
-      <c r="D26" s="13"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="14"/>
       <c r="E26" s="4" t="s">
         <v>11</v>
       </c>
@@ -13918,8 +13766,8 @@
     </row>
     <row r="27" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B27" s="2"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="12" t="s">
+      <c r="C27" s="11"/>
+      <c r="D27" s="13" t="s">
         <v>26</v>
       </c>
       <c r="E27" s="4" t="s">
@@ -13948,8 +13796,8 @@
     </row>
     <row r="28" spans="2:14" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B28" s="2"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="13"/>
+      <c r="C28" s="11"/>
+      <c r="D28" s="14"/>
       <c r="E28" s="4" t="s">
         <v>11</v>
       </c>
@@ -14171,6 +14019,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="C5:C8"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="C3:E3"/>
     <mergeCell ref="F3:J3"/>
     <mergeCell ref="C9:C12"/>
     <mergeCell ref="C17:C20"/>
@@ -14187,10 +14039,6 @@
     <mergeCell ref="D25:D26"/>
     <mergeCell ref="D13:D14"/>
     <mergeCell ref="D23:D24"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="C5:C8"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="C3:E3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -14248,13 +14096,13 @@
       </c>
       <c r="K1" s="7"/>
       <c r="L1" s="7" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="M1" s="7" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="N1" s="7" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="O1" s="7" t="s">
         <v>7</v>
@@ -20485,7 +20333,7 @@
   <dimension ref="B2:M28"/>
   <sheetViews>
     <sheetView zoomScale="157" zoomScaleNormal="136" workbookViewId="0">
-      <selection activeCell="L8" sqref="L8"/>
+      <selection activeCell="E4" sqref="E4:F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -20498,17 +20346,17 @@
   <sheetData>
     <row r="2" spans="2:13" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B2" s="2"/>
-      <c r="C2" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="14"/>
-      <c r="E2" s="15" t="s">
+      <c r="C2" s="12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2" s="12"/>
+      <c r="E2" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="F2" s="15"/>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-      <c r="I2" s="15"/>
+      <c r="F2" s="11"/>
+      <c r="G2" s="11"/>
+      <c r="H2" s="11"/>
+      <c r="I2" s="11"/>
       <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
@@ -20544,7 +20392,7 @@
     </row>
     <row r="4" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
-      <c r="C4" s="14" t="s">
+      <c r="C4" s="12" t="s">
         <v>23</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -20577,7 +20425,7 @@
     </row>
     <row r="5" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
-      <c r="C5" s="15"/>
+      <c r="C5" s="11"/>
       <c r="D5" s="4" t="s">
         <v>11</v>
       </c>
@@ -20608,7 +20456,7 @@
     </row>
     <row r="6" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="14" t="s">
+      <c r="C6" s="12" t="s">
         <v>36</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -20641,7 +20489,7 @@
     </row>
     <row r="7" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="C7" s="15"/>
+      <c r="C7" s="11"/>
       <c r="D7" s="4" t="s">
         <v>11</v>
       </c>
@@ -20672,7 +20520,7 @@
     </row>
     <row r="8" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="11" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -20705,7 +20553,7 @@
     </row>
     <row r="9" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="C9" s="15"/>
+      <c r="C9" s="11"/>
       <c r="D9" s="4" t="s">
         <v>11</v>
       </c>
@@ -20736,7 +20584,7 @@
     </row>
     <row r="10" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="12" t="s">
         <v>38</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -20769,7 +20617,7 @@
     </row>
     <row r="11" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="C11" s="15"/>
+      <c r="C11" s="11"/>
       <c r="D11" s="4" t="s">
         <v>11</v>
       </c>
@@ -20800,7 +20648,7 @@
     </row>
     <row r="12" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="11" t="s">
         <v>25</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -20833,7 +20681,7 @@
     </row>
     <row r="13" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="15"/>
+      <c r="C13" s="11"/>
       <c r="D13" s="4" t="s">
         <v>11</v>
       </c>
@@ -20864,7 +20712,7 @@
     </row>
     <row r="14" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="12" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -20897,7 +20745,7 @@
     </row>
     <row r="15" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="15"/>
+      <c r="C15" s="11"/>
       <c r="D15" s="4" t="s">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
Remove SL library from LTMLE, does not help
</commit_message>
<xml_diff>
--- a/results/Paper/table_4.xlsx
+++ b/results/Paper/table_4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\João Matos\Documents\Education\MIT\Projects\Race Disparities in Sepsis\mit-tmle\results\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0B4A4AF-0ED7-4C5D-80AF-4709C755C648}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F622E18A-5669-4122-B0D8-56F04FD88D26}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -770,7 +770,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -797,12 +797,6 @@
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -834,25 +828,25 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="16" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="16" fontId="21" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="16" fontId="22" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -11288,17 +11282,17 @@
   <sheetData>
     <row r="3" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B3" s="2"/>
-      <c r="C3" s="14" t="s">
+      <c r="C3" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="13" t="s">
+      <c r="D3" s="27"/>
+      <c r="E3" s="26" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
+      <c r="F3" s="26"/>
+      <c r="G3" s="26"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
       <c r="J3" s="2"/>
       <c r="K3" s="2"/>
       <c r="L3" s="2"/>
@@ -11334,7 +11328,7 @@
     </row>
     <row r="5" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="26" t="s">
         <v>21</v>
       </c>
       <c r="D5" s="12" t="s">
@@ -11363,7 +11357,7 @@
     </row>
     <row r="6" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="C6" s="13"/>
+      <c r="C6" s="26"/>
       <c r="D6" s="12" t="s">
         <v>46</v>
       </c>
@@ -11390,7 +11384,7 @@
     </row>
     <row r="7" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
-      <c r="C7" s="14" t="s">
+      <c r="C7" s="27" t="s">
         <v>33</v>
       </c>
       <c r="D7" s="12" t="s">
@@ -11419,7 +11413,7 @@
     </row>
     <row r="8" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
-      <c r="C8" s="13"/>
+      <c r="C8" s="26"/>
       <c r="D8" s="12" t="s">
         <v>46</v>
       </c>
@@ -11446,7 +11440,7 @@
     </row>
     <row r="9" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B9" s="2"/>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="26" t="s">
         <v>22</v>
       </c>
       <c r="D9" s="12" t="s">
@@ -11475,7 +11469,7 @@
     </row>
     <row r="10" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B10" s="2"/>
-      <c r="C10" s="13"/>
+      <c r="C10" s="26"/>
       <c r="D10" s="12" t="s">
         <v>46</v>
       </c>
@@ -11502,7 +11496,7 @@
     </row>
     <row r="11" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B11" s="2"/>
-      <c r="C11" s="14" t="s">
+      <c r="C11" s="27" t="s">
         <v>34</v>
       </c>
       <c r="D11" s="12" t="s">
@@ -11531,7 +11525,7 @@
     </row>
     <row r="12" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B12" s="2"/>
-      <c r="C12" s="13"/>
+      <c r="C12" s="26"/>
       <c r="D12" s="12" t="s">
         <v>46</v>
       </c>
@@ -11558,7 +11552,7 @@
     </row>
     <row r="13" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B13" s="2"/>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="26" t="s">
         <v>23</v>
       </c>
       <c r="D13" s="12" t="s">
@@ -11587,7 +11581,7 @@
     </row>
     <row r="14" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B14" s="2"/>
-      <c r="C14" s="13"/>
+      <c r="C14" s="26"/>
       <c r="D14" s="12" t="s">
         <v>46</v>
       </c>
@@ -11614,7 +11608,7 @@
     </row>
     <row r="15" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B15" s="2"/>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="27" t="s">
         <v>35</v>
       </c>
       <c r="D15" s="12" t="s">
@@ -11643,7 +11637,7 @@
     </row>
     <row r="16" spans="2:13" ht="19.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B16" s="2"/>
-      <c r="C16" s="13"/>
+      <c r="C16" s="26"/>
       <c r="D16" s="12" t="s">
         <v>46</v>
       </c>
@@ -11852,14 +11846,14 @@
     </row>
   </sheetData>
   <mergeCells count="8">
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="C13:C14"/>
+    <mergeCell ref="C9:C10"/>
     <mergeCell ref="C5:C6"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="E3:I3"/>
     <mergeCell ref="C7:C8"/>
     <mergeCell ref="C11:C12"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="C13:C14"/>
-    <mergeCell ref="C9:C10"/>
   </mergeCells>
   <phoneticPr fontId="20" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -11871,735 +11865,723 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E5414F4A-3CCF-48B8-9041-E473F806DC9D}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView tabSelected="1" zoomScale="128" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="2" style="15" customWidth="1"/>
-    <col min="2" max="2" width="9.77734375" style="17" customWidth="1"/>
-    <col min="3" max="4" width="17.44140625" style="15" customWidth="1"/>
-    <col min="5" max="5" width="2" style="15" customWidth="1"/>
-    <col min="6" max="6" width="9.77734375" style="17" customWidth="1"/>
-    <col min="7" max="8" width="17.44140625" style="15" customWidth="1"/>
-    <col min="9" max="9" width="2" style="15" customWidth="1"/>
-    <col min="10" max="10" width="9.77734375" style="17" customWidth="1"/>
-    <col min="11" max="12" width="17.44140625" style="15" customWidth="1"/>
-    <col min="13" max="13" width="2" style="15" customWidth="1"/>
-    <col min="14" max="14" width="9.77734375" style="17" customWidth="1"/>
-    <col min="15" max="16" width="17.44140625" style="15" customWidth="1"/>
-    <col min="17" max="17" width="2" style="15" customWidth="1"/>
-    <col min="18" max="18" width="9.77734375" style="17" customWidth="1"/>
-    <col min="19" max="20" width="17.44140625" style="15" customWidth="1"/>
-    <col min="21" max="21" width="2" style="15" customWidth="1"/>
-    <col min="22" max="16384" width="8.88671875" style="16"/>
+    <col min="1" max="1" width="2" style="13" customWidth="1"/>
+    <col min="2" max="2" width="9.77734375" style="15" customWidth="1"/>
+    <col min="3" max="4" width="17.44140625" style="13" customWidth="1"/>
+    <col min="5" max="5" width="2" style="13" customWidth="1"/>
+    <col min="6" max="6" width="9.77734375" style="15" customWidth="1"/>
+    <col min="7" max="8" width="17.44140625" style="13" customWidth="1"/>
+    <col min="9" max="9" width="2" style="13" customWidth="1"/>
+    <col min="10" max="10" width="9.77734375" style="15" customWidth="1"/>
+    <col min="11" max="12" width="17.44140625" style="13" customWidth="1"/>
+    <col min="13" max="13" width="2" style="13" customWidth="1"/>
+    <col min="14" max="14" width="9.77734375" style="15" customWidth="1"/>
+    <col min="15" max="16" width="17.44140625" style="13" customWidth="1"/>
+    <col min="17" max="17" width="2" style="13" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" style="15" customWidth="1"/>
+    <col min="19" max="20" width="17.44140625" style="13" customWidth="1"/>
+    <col min="21" max="21" width="2" style="13" customWidth="1"/>
+    <col min="22" max="16384" width="8.88671875" style="14"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="J1" s="18"/>
-      <c r="L1" s="22"/>
-      <c r="N1" s="18"/>
-      <c r="P1" s="22"/>
-      <c r="R1" s="18"/>
-      <c r="T1" s="22"/>
-    </row>
-    <row r="2" spans="1:21" s="20" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="27"/>
-      <c r="B2" s="23" t="s">
+      <c r="B1" s="16"/>
+      <c r="F1" s="16"/>
+      <c r="J1" s="16"/>
+      <c r="L1" s="20"/>
+      <c r="N1" s="16"/>
+      <c r="P1" s="20"/>
+      <c r="R1" s="16"/>
+      <c r="T1" s="20"/>
+    </row>
+    <row r="2" spans="1:21" s="18" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="17"/>
+      <c r="B2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C2" s="24" t="str">
+      <c r="C2" s="28" t="str">
         <f>table_4!E4</f>
         <v>All</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="23" t="s">
+      <c r="D2" s="28"/>
+      <c r="E2" s="17"/>
+      <c r="F2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G2" s="24" t="str">
+      <c r="G2" s="28" t="str">
         <f>table_4!F4</f>
         <v>0 - 5</v>
       </c>
-      <c r="H2" s="24"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="23" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="21" t="s">
         <v>51</v>
       </c>
       <c r="K2" s="29" t="str">
         <f>table_4!G4</f>
         <v>6 - 10</v>
       </c>
-      <c r="L2" s="24"/>
-      <c r="M2" s="27"/>
-      <c r="N2" s="23" t="s">
+      <c r="L2" s="28"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="O2" s="24" t="str">
+      <c r="O2" s="28" t="str">
         <f>table_4!H4</f>
         <v>11 - 15</v>
       </c>
-      <c r="P2" s="24"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="23" t="s">
+      <c r="P2" s="28"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="S2" s="24" t="str">
+      <c r="S2" s="28" t="str">
         <f>table_4!I4</f>
         <v>&gt; 15</v>
       </c>
-      <c r="T2" s="24"/>
-      <c r="U2" s="27"/>
-    </row>
-    <row r="3" spans="1:21" s="21" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="27"/>
-      <c r="B3" s="23" t="s">
+      <c r="T2" s="28"/>
+      <c r="U2" s="17"/>
+    </row>
+    <row r="3" spans="1:21" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="17"/>
+      <c r="B3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="D3" s="25" t="s">
+      <c r="D3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="17"/>
+      <c r="F3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G3" s="25" t="s">
+      <c r="G3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="H3" s="25" t="s">
+      <c r="H3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="I3" s="27"/>
-      <c r="J3" s="23" t="s">
+      <c r="I3" s="17"/>
+      <c r="J3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K3" s="25" t="s">
+      <c r="K3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="L3" s="25" t="s">
+      <c r="L3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="M3" s="27"/>
-      <c r="N3" s="23" t="s">
+      <c r="M3" s="17"/>
+      <c r="N3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="O3" s="25" t="s">
+      <c r="O3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="P3" s="25" t="s">
+      <c r="P3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="Q3" s="27"/>
-      <c r="R3" s="23" t="s">
+      <c r="Q3" s="17"/>
+      <c r="R3" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="S3" s="25" t="s">
+      <c r="S3" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="T3" s="25" t="s">
+      <c r="T3" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="U3" s="27"/>
+      <c r="U3" s="17"/>
     </row>
     <row r="4" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="28"/>
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="26" t="str">
+      <c r="C4" s="23" t="str">
         <f>table_4!E8</f>
         <v>0.246 (0.241 - 0.251)*</v>
       </c>
-      <c r="D4" s="26" t="str">
+      <c r="D4" s="23" t="str">
         <f>table_4!E6</f>
         <v>0.346 (0.340 - 0.353)*</v>
       </c>
-      <c r="E4" s="28"/>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="26" t="str">
+      <c r="G4" s="23" t="str">
         <f>table_4!F8</f>
         <v>0.190 (0.185 - 0.195)*</v>
       </c>
-      <c r="H4" s="26" t="str">
+      <c r="H4" s="23" t="str">
         <f>table_4!F6</f>
         <v>0.227 (0.218 - 0.235)*</v>
       </c>
-      <c r="I4" s="28"/>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K4" s="26" t="str">
+      <c r="K4" s="23" t="str">
         <f>table_4!G8</f>
         <v>0.383 (0.371 - 0.394)*</v>
       </c>
-      <c r="L4" s="30" t="str">
+      <c r="L4" s="24" t="str">
         <f>table_4!G6</f>
         <v>0.363 (0.353 - 0.373)*</v>
       </c>
-      <c r="M4" s="28"/>
-      <c r="N4" s="23" t="s">
+      <c r="N4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O4" s="26" t="str">
+      <c r="O4" s="23" t="str">
         <f>table_4!H8</f>
         <v>0.679 (0.642 - 0.715)*</v>
       </c>
-      <c r="P4" s="30" t="str">
+      <c r="P4" s="24" t="str">
         <f>table_4!H6</f>
         <v>0.583 (0.566 - 0.600)*</v>
       </c>
-      <c r="Q4" s="28"/>
-      <c r="R4" s="23" t="s">
+      <c r="R4" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="S4" s="26" t="str">
+      <c r="S4" s="23" t="str">
         <f>table_4!I8</f>
         <v>0.889 (0.770 - 1.000)*</v>
       </c>
-      <c r="T4" s="30" t="str">
+      <c r="T4" s="24" t="str">
         <f>table_4!I6</f>
         <v>0.738 (0.700 - 0.776)*</v>
       </c>
-      <c r="U4" s="28"/>
     </row>
     <row r="5" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="28"/>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C5" s="26" t="str">
+      <c r="C5" s="23" t="str">
         <f>table_4!E7</f>
         <v>0.268 (0.258 - 0.278)*</v>
       </c>
-      <c r="D5" s="26" t="str">
+      <c r="D5" s="23" t="str">
         <f>table_4!E5</f>
         <v>0.374 (0.361 - 0.387)*</v>
       </c>
-      <c r="E5" s="28"/>
-      <c r="F5" s="23" t="s">
+      <c r="F5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G5" s="26" t="str">
+      <c r="G5" s="23" t="str">
         <f>table_4!F7</f>
         <v>0.202 (0.191 - 0.213)*</v>
       </c>
-      <c r="H5" s="26" t="str">
+      <c r="H5" s="23" t="str">
         <f>table_4!F5</f>
         <v>0.233 (0.215 - 0.252)*</v>
       </c>
-      <c r="I5" s="28"/>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K5" s="26" t="str">
+      <c r="K5" s="23" t="str">
         <f>table_4!G7</f>
         <v>0.389 (0.368 - 0.410)*</v>
       </c>
-      <c r="L5" s="30" t="str">
+      <c r="L5" s="24" t="str">
         <f>table_4!G5</f>
         <v>0.389 (0.369 - 0.410)*</v>
       </c>
-      <c r="M5" s="28"/>
-      <c r="N5" s="23" t="s">
+      <c r="N5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O5" s="26" t="str">
+      <c r="O5" s="23" t="str">
         <f>table_4!H7</f>
         <v>0.680 (0.611 - 0.750)*</v>
       </c>
-      <c r="P5" s="30" t="str">
+      <c r="P5" s="24" t="str">
         <f>table_4!H5</f>
         <v>0.592 (0.560 - 0.624)*</v>
       </c>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="23" t="s">
+      <c r="R5" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="S5" s="26" t="str">
+      <c r="S5" s="23" t="str">
         <f>table_4!I7</f>
         <v>0.800 (0.552 - 1.000)*</v>
       </c>
-      <c r="T5" s="30" t="str">
+      <c r="T5" s="24" t="str">
         <f>table_4!I5</f>
         <v>0.710 (0.638 - 0.781)*</v>
       </c>
-      <c r="U5" s="28"/>
     </row>
     <row r="6" spans="1:21" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="J6" s="18"/>
-      <c r="L6" s="22"/>
-      <c r="N6" s="18"/>
-      <c r="P6" s="22"/>
-      <c r="R6" s="18"/>
-      <c r="T6" s="22"/>
-    </row>
-    <row r="7" spans="1:21" s="21" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="19"/>
-      <c r="B7" s="23" t="s">
+      <c r="B6" s="16"/>
+      <c r="F6" s="16"/>
+      <c r="J6" s="16"/>
+      <c r="L6" s="20"/>
+      <c r="N6" s="16"/>
+      <c r="P6" s="20"/>
+      <c r="R6" s="16"/>
+      <c r="T6" s="20"/>
+    </row>
+    <row r="7" spans="1:21" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="17"/>
+      <c r="B7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D7" s="24"/>
-      <c r="E7" s="19"/>
-      <c r="F7" s="23" t="s">
+      <c r="D7" s="28"/>
+      <c r="E7" s="17"/>
+      <c r="F7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="I7" s="19"/>
-      <c r="J7" s="23" t="s">
+      <c r="H7" s="28"/>
+      <c r="I7" s="17"/>
+      <c r="J7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L7" s="24"/>
-      <c r="M7" s="19"/>
-      <c r="N7" s="23" t="s">
+      <c r="L7" s="28"/>
+      <c r="M7" s="17"/>
+      <c r="N7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="P7" s="24"/>
-      <c r="Q7" s="19"/>
-      <c r="R7" s="23" t="s">
+      <c r="P7" s="28"/>
+      <c r="Q7" s="17"/>
+      <c r="R7" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="T7" s="24"/>
-      <c r="U7" s="19"/>
-    </row>
-    <row r="8" spans="1:21" s="21" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="19"/>
-      <c r="B8" s="23" t="s">
+      <c r="T7" s="28"/>
+      <c r="U7" s="17"/>
+    </row>
+    <row r="8" spans="1:21" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="17"/>
+      <c r="B8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C8" s="25" t="s">
+      <c r="C8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="E8" s="19"/>
-      <c r="F8" s="23" t="s">
+      <c r="E8" s="17"/>
+      <c r="F8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="25" t="s">
+      <c r="G8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="H8" s="25" t="s">
+      <c r="H8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="I8" s="19"/>
-      <c r="J8" s="23" t="s">
+      <c r="I8" s="17"/>
+      <c r="J8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K8" s="25" t="s">
+      <c r="K8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="L8" s="25" t="s">
+      <c r="L8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="23" t="s">
+      <c r="M8" s="17"/>
+      <c r="N8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="O8" s="25" t="s">
+      <c r="O8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="P8" s="25" t="s">
+      <c r="P8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q8" s="19"/>
-      <c r="R8" s="23" t="s">
+      <c r="Q8" s="17"/>
+      <c r="R8" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="S8" s="25" t="s">
+      <c r="S8" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="T8" s="25" t="s">
+      <c r="T8" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="U8" s="19"/>
+      <c r="U8" s="17"/>
     </row>
     <row r="9" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="23" t="s">
+      <c r="B9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="26" t="str">
+      <c r="C9" s="23" t="str">
         <f>table_4!E12</f>
         <v>0.274 (0.270 - 0.278)*</v>
       </c>
-      <c r="D9" s="26" t="str">
+      <c r="D9" s="23" t="str">
         <f>table_4!E10</f>
         <v>0.459 (0.444 - 0.474)*</v>
       </c>
-      <c r="F9" s="23" t="s">
+      <c r="F9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G9" s="26" t="str">
+      <c r="G9" s="23" t="str">
         <f>table_4!F12</f>
         <v>0.198 (0.194 - 0.203)*</v>
       </c>
-      <c r="H9" s="26" t="str">
+      <c r="H9" s="23" t="str">
         <f>table_4!F10</f>
         <v>0.286 (0.258 - 0.313)*</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K9" s="26" t="str">
+      <c r="K9" s="23" t="str">
         <f>table_4!G12</f>
         <v>0.362 (0.354 - 0.370)*</v>
       </c>
-      <c r="L9" s="26" t="str">
+      <c r="L9" s="23" t="str">
         <f>table_4!G10</f>
         <v>0.446 (0.423 - 0.469)*</v>
       </c>
-      <c r="N9" s="23" t="s">
+      <c r="N9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O9" s="26" t="str">
+      <c r="O9" s="23" t="str">
         <f>table_4!H12</f>
         <v>0.603 (0.585 - 0.621)*</v>
       </c>
-      <c r="P9" s="26" t="str">
+      <c r="P9" s="23" t="str">
         <f>table_4!H10</f>
         <v>0.588 (0.557 - 0.618)*</v>
       </c>
-      <c r="R9" s="23" t="s">
+      <c r="R9" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="S9" s="26" t="str">
+      <c r="S9" s="23" t="str">
         <f>table_4!I12</f>
         <v>0.802 (0.754 - 0.850)*</v>
       </c>
-      <c r="T9" s="26" t="str">
+      <c r="T9" s="23" t="str">
         <f>table_4!I10</f>
         <v>0.693 (0.640 - 0.747)*</v>
       </c>
     </row>
     <row r="10" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="23" t="s">
+      <c r="B10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C10" s="26" t="str">
+      <c r="C10" s="23" t="str">
         <f>table_4!E11</f>
         <v>0.291 (0.282 - 0.299)*</v>
       </c>
-      <c r="D10" s="26" t="str">
+      <c r="D10" s="23" t="str">
         <f>table_4!E9</f>
         <v>0.443 (0.420 - 0.466)*</v>
       </c>
-      <c r="F10" s="23" t="s">
+      <c r="F10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G10" s="26" t="str">
+      <c r="G10" s="23" t="str">
         <f>table_4!F11</f>
         <v>0.206 (0.196 - 0.216)*</v>
       </c>
-      <c r="H10" s="26" t="str">
+      <c r="H10" s="23" t="str">
         <f>table_4!F9</f>
         <v>0.284 (0.242 - 0.327)*</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K10" s="26" t="str">
+      <c r="K10" s="23" t="str">
         <f>table_4!G11</f>
         <v>0.377 (0.361 - 0.393)*</v>
       </c>
-      <c r="L10" s="26" t="str">
+      <c r="L10" s="23" t="str">
         <f>table_4!G9</f>
         <v>0.437 (0.404 - 0.469)*</v>
       </c>
-      <c r="N10" s="23" t="s">
+      <c r="N10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O10" s="26" t="str">
+      <c r="O10" s="23" t="str">
         <f>table_4!H11</f>
         <v>0.609 (0.575 - 0.644)*</v>
       </c>
-      <c r="P10" s="26" t="str">
+      <c r="P10" s="23" t="str">
         <f>table_4!H9</f>
         <v>0.598 (0.546 - 0.651)*</v>
       </c>
-      <c r="R10" s="23" t="s">
+      <c r="R10" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="S10" s="26" t="str">
+      <c r="S10" s="23" t="str">
         <f>table_4!I11</f>
         <v>0.767 (0.670 - 0.864)*</v>
       </c>
-      <c r="T10" s="26" t="str">
+      <c r="T10" s="23" t="str">
         <f>table_4!I9</f>
         <v>0.674 (0.578 - 0.770)*</v>
       </c>
     </row>
     <row r="11" spans="1:21" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="J11" s="18"/>
-      <c r="N11" s="18"/>
-      <c r="R11" s="18"/>
+      <c r="B11" s="16"/>
+      <c r="F11" s="16"/>
+      <c r="J11" s="16"/>
+      <c r="N11" s="16"/>
+      <c r="R11" s="16"/>
     </row>
     <row r="12" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="19"/>
-      <c r="B12" s="23" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="D12" s="24"/>
-      <c r="E12" s="19"/>
-      <c r="F12" s="23" t="s">
+      <c r="D12" s="28"/>
+      <c r="E12" s="17"/>
+      <c r="F12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="28" t="s">
         <v>30</v>
       </c>
-      <c r="H12" s="24"/>
-      <c r="I12" s="19"/>
-      <c r="J12" s="23" t="s">
+      <c r="H12" s="28"/>
+      <c r="I12" s="17"/>
+      <c r="J12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="K12" s="28" t="s">
         <v>25</v>
       </c>
-      <c r="L12" s="24"/>
-      <c r="M12" s="19"/>
-      <c r="N12" s="23" t="s">
+      <c r="L12" s="28"/>
+      <c r="M12" s="17"/>
+      <c r="N12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="O12" s="24" t="s">
+      <c r="O12" s="28" t="s">
         <v>26</v>
       </c>
-      <c r="P12" s="24"/>
-      <c r="Q12" s="19"/>
-      <c r="R12" s="23" t="s">
+      <c r="P12" s="28"/>
+      <c r="Q12" s="17"/>
+      <c r="R12" s="21" t="s">
         <v>51</v>
       </c>
-      <c r="S12" s="24" t="s">
+      <c r="S12" s="28" t="s">
         <v>31</v>
       </c>
-      <c r="T12" s="24"/>
-      <c r="U12" s="19"/>
-    </row>
-    <row r="13" spans="1:21" s="21" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="19"/>
-      <c r="B13" s="23" t="s">
+      <c r="T12" s="28"/>
+      <c r="U12" s="17"/>
+    </row>
+    <row r="13" spans="1:21" s="19" customFormat="1" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="C13" s="25" t="s">
+      <c r="C13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D13" s="25" t="s">
+      <c r="D13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="23" t="s">
+      <c r="E13" s="17"/>
+      <c r="F13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="25" t="s">
+      <c r="G13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="H13" s="25" t="s">
+      <c r="H13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="I13" s="19"/>
-      <c r="J13" s="23" t="s">
+      <c r="I13" s="17"/>
+      <c r="J13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="K13" s="25" t="s">
+      <c r="K13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="L13" s="25" t="s">
+      <c r="L13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="M13" s="19"/>
-      <c r="N13" s="23" t="s">
+      <c r="M13" s="17"/>
+      <c r="N13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="O13" s="25" t="s">
+      <c r="O13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="P13" s="25" t="s">
+      <c r="P13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="Q13" s="19"/>
-      <c r="R13" s="23" t="s">
+      <c r="Q13" s="17"/>
+      <c r="R13" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="S13" s="25" t="s">
+      <c r="S13" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="T13" s="25" t="s">
+      <c r="T13" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="U13" s="19"/>
+      <c r="U13" s="17"/>
     </row>
     <row r="14" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="23" t="s">
+      <c r="B14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="C14" s="26" t="str">
+      <c r="C14" s="23" t="str">
         <f>table_4!E16</f>
         <v>0.233 (0.228 - 0.238)*</v>
       </c>
-      <c r="D14" s="26" t="str">
+      <c r="D14" s="23" t="str">
         <f>table_4!E14</f>
         <v>0.354 (0.348 - 0.360)*</v>
       </c>
-      <c r="F14" s="23" t="s">
+      <c r="F14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="G14" s="26" t="str">
+      <c r="G14" s="23" t="str">
         <f>table_4!F16</f>
         <v>0.192 (0.187 - 0.197)*</v>
       </c>
-      <c r="H14" s="26" t="str">
+      <c r="H14" s="23" t="str">
         <f>table_4!F14</f>
         <v>0.220 (0.212 - 0.228)*</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="K14" s="26" t="str">
+      <c r="K14" s="23" t="str">
         <f>table_4!G16</f>
         <v>0.362 (0.350 - 0.374)*</v>
       </c>
-      <c r="L14" s="26" t="str">
+      <c r="L14" s="23" t="str">
         <f>table_4!G14</f>
         <v>0.377 (0.368 - 0.387)*</v>
       </c>
-      <c r="N14" s="23" t="s">
+      <c r="N14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="O14" s="26" t="str">
+      <c r="O14" s="23" t="str">
         <f>table_4!H16</f>
         <v>0.546 (0.495 - 0.597)*</v>
       </c>
-      <c r="P14" s="26" t="str">
+      <c r="P14" s="23" t="str">
         <f>table_4!H14</f>
         <v>0.604 (0.588 - 0.621)*</v>
       </c>
-      <c r="R14" s="23" t="s">
+      <c r="R14" s="21" t="s">
         <v>46</v>
       </c>
-      <c r="S14" s="31" t="str">
+      <c r="S14" s="25" t="str">
         <f>table_4!I16</f>
         <v xml:space="preserve">0.000 (0.000 - 0.000) </v>
       </c>
-      <c r="T14" s="26" t="str">
+      <c r="T14" s="23" t="str">
         <f>table_4!I14</f>
         <v>0.744 (0.707 - 0.781)*</v>
       </c>
     </row>
     <row r="15" spans="1:21" ht="19.8" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="23" t="s">
+      <c r="B15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="C15" s="26" t="str">
+      <c r="C15" s="23" t="str">
         <f>table_4!E15</f>
         <v>0.259 (0.249 - 0.269)*</v>
       </c>
-      <c r="D15" s="26" t="str">
+      <c r="D15" s="23" t="str">
         <f>table_4!E13</f>
         <v>0.386 (0.373 - 0.399)*</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="G15" s="26" t="str">
+      <c r="G15" s="23" t="str">
         <f>table_4!F15</f>
         <v>0.206 (0.195 - 0.217)*</v>
       </c>
-      <c r="H15" s="26" t="str">
+      <c r="H15" s="23" t="str">
         <f>table_4!F13</f>
         <v>0.223 (0.204 - 0.243)*</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="K15" s="26" t="str">
+      <c r="K15" s="23" t="str">
         <f>table_4!G15</f>
         <v>0.384 (0.363 - 0.406)*</v>
       </c>
-      <c r="L15" s="26" t="str">
+      <c r="L15" s="23" t="str">
         <f>table_4!G13</f>
         <v>0.393 (0.373 - 0.413)*</v>
       </c>
-      <c r="N15" s="23" t="s">
+      <c r="N15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="O15" s="26" t="str">
+      <c r="O15" s="23" t="str">
         <f>table_4!H15</f>
         <v>0.469 (0.382 - 0.555)*</v>
       </c>
-      <c r="P15" s="26" t="str">
+      <c r="P15" s="23" t="str">
         <f>table_4!H13</f>
         <v>0.624 (0.594 - 0.655)*</v>
       </c>
-      <c r="R15" s="23" t="s">
+      <c r="R15" s="21" t="s">
         <v>24</v>
       </c>
-      <c r="S15" s="31" t="str">
+      <c r="S15" s="25" t="str">
         <f>table_4!I15</f>
         <v xml:space="preserve">0.000 (0.000 - 0.000) </v>
       </c>
-      <c r="T15" s="26" t="str">
+      <c r="T15" s="23" t="str">
         <f>table_4!I13</f>
         <v>0.716 (0.647 - 0.786)*</v>
       </c>
     </row>
     <row r="16" spans="1:21" ht="7.95" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="J16" s="18"/>
-      <c r="L16" s="22"/>
-      <c r="N16" s="18"/>
-      <c r="P16" s="22"/>
-      <c r="R16" s="18"/>
-      <c r="T16" s="22"/>
+      <c r="B16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="L16" s="20"/>
+      <c r="N16" s="16"/>
+      <c r="P16" s="20"/>
+      <c r="R16" s="16"/>
+      <c r="T16" s="20"/>
     </row>
     <row r="17" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="18" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="19" ht="19.8" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="15">
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="K2:L2"/>
+    <mergeCell ref="O2:P2"/>
+    <mergeCell ref="S2:T2"/>
+    <mergeCell ref="C12:D12"/>
+    <mergeCell ref="G12:H12"/>
+    <mergeCell ref="K12:L12"/>
+    <mergeCell ref="O12:P12"/>
+    <mergeCell ref="S12:T12"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="G7:H7"/>
     <mergeCell ref="K7:L7"/>
     <mergeCell ref="O7:P7"/>
     <mergeCell ref="S7:T7"/>
-    <mergeCell ref="C12:D12"/>
-    <mergeCell ref="G12:H12"/>
-    <mergeCell ref="K12:L12"/>
-    <mergeCell ref="O12:P12"/>
-    <mergeCell ref="S12:T12"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="K2:L2"/>
-    <mergeCell ref="O2:P2"/>
-    <mergeCell ref="S2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>